<commit_message>
Updated the AuditLogs Script
</commit_message>
<xml_diff>
--- a/tests/artifact/script/UI-AuditLogs.xlsx
+++ b/tests/artifact/script/UI-AuditLogs.xlsx
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="832">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="834">
   <si>
     <t>target</t>
   </si>
@@ -2486,7 +2486,13 @@
     <t>Verify already Entered From date</t>
   </si>
   <si>
+    <t>Verify the value is not presenting in From date</t>
+  </si>
+  <si>
     <t>Verify already Entered To date</t>
+  </si>
+  <si>
+    <t>Verify the value is not presenting in To date</t>
   </si>
   <si>
     <t>Click on Filter option</t>
@@ -3314,7 +3320,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3458,6 +3464,10 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="58" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -6652,14 +6662,14 @@
       <c r="I1" s="15" t="s">
         <v>731</v>
       </c>
-      <c r="J1" s="43"/>
+      <c r="J1" s="44"/>
       <c r="K1" s="23"/>
       <c r="L1" s="15" t="s">
         <v>732</v>
       </c>
       <c r="M1" s="15"/>
       <c r="N1" s="15"/>
-      <c r="O1" s="44"/>
+      <c r="O1" s="45"/>
     </row>
     <row r="2" s="1" customFormat="1" ht="15.25" spans="1:15">
       <c r="A2" s="16" t="s">
@@ -6673,12 +6683,12 @@
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
       <c r="I2" s="19"/>
-      <c r="J2" s="43"/>
+      <c r="J2" s="44"/>
       <c r="K2" s="23"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
     </row>
     <row r="3" s="1" customFormat="1" ht="10" customHeight="1" spans="1:15">
       <c r="A3" s="20"/>
@@ -6690,7 +6700,7 @@
       <c r="G3" s="24"/>
       <c r="H3" s="24"/>
       <c r="I3" s="24"/>
-      <c r="J3" s="47"/>
+      <c r="J3" s="48"/>
       <c r="K3" s="23"/>
       <c r="L3" s="24"/>
       <c r="M3" s="22"/>
@@ -6725,10 +6735,10 @@
       <c r="I4" s="25" t="s">
         <v>741</v>
       </c>
-      <c r="J4" s="48" t="s">
+      <c r="J4" s="49" t="s">
         <v>742</v>
       </c>
-      <c r="K4" s="49"/>
+      <c r="K4" s="50"/>
       <c r="L4" s="25" t="s">
         <v>743</v>
       </c>
@@ -6743,7 +6753,7 @@
       </c>
     </row>
     <row r="5" s="3" customFormat="1" ht="40" customHeight="1" spans="1:15">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="60" t="s">
         <v>747</v>
       </c>
       <c r="B5" s="31" t="s">
@@ -6758,69 +6768,69 @@
       <c r="E5" s="33" t="s">
         <v>749</v>
       </c>
-      <c r="F5" s="60" t="s">
+      <c r="F5" s="61" t="s">
         <v>750</v>
       </c>
       <c r="G5" s="28"/>
       <c r="H5" s="30"/>
       <c r="I5" s="30"/>
-      <c r="J5" s="50"/>
-      <c r="K5" s="51"/>
-      <c r="L5" s="52"/>
-      <c r="M5" s="53"/>
-      <c r="N5" s="52"/>
-      <c r="O5" s="51"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="52"/>
+      <c r="L5" s="53"/>
+      <c r="M5" s="54"/>
+      <c r="N5" s="53"/>
+      <c r="O5" s="52"/>
     </row>
     <row r="6" s="3" customFormat="1" ht="19" customHeight="1" spans="1:15">
-      <c r="A6" s="61"/>
-      <c r="B6" s="62"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="64"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="65"/>
-      <c r="G6" s="64"/>
+      <c r="A6" s="62"/>
+      <c r="B6" s="63"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="65"/>
       <c r="H6" s="30"/>
       <c r="I6" s="30"/>
-      <c r="J6" s="50"/>
-      <c r="K6" s="51"/>
-      <c r="L6" s="52"/>
-      <c r="M6" s="53"/>
-      <c r="N6" s="52"/>
-      <c r="O6" s="51"/>
+      <c r="J6" s="51"/>
+      <c r="K6" s="52"/>
+      <c r="L6" s="53"/>
+      <c r="M6" s="54"/>
+      <c r="N6" s="53"/>
+      <c r="O6" s="52"/>
     </row>
     <row r="7" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A7" s="61"/>
-      <c r="B7" s="62"/>
-      <c r="C7" s="66"/>
+      <c r="A7" s="62"/>
+      <c r="B7" s="63"/>
+      <c r="C7" s="67"/>
       <c r="D7" s="30"/>
       <c r="E7" s="30"/>
       <c r="F7" s="30"/>
       <c r="G7" s="30"/>
       <c r="H7" s="30"/>
       <c r="I7" s="30"/>
-      <c r="J7" s="50"/>
-      <c r="K7" s="51"/>
-      <c r="L7" s="52"/>
-      <c r="M7" s="53"/>
-      <c r="N7" s="52"/>
-      <c r="O7" s="51"/>
+      <c r="J7" s="51"/>
+      <c r="K7" s="52"/>
+      <c r="L7" s="53"/>
+      <c r="M7" s="54"/>
+      <c r="N7" s="53"/>
+      <c r="O7" s="52"/>
     </row>
     <row r="8" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A8" s="61"/>
-      <c r="B8" s="62"/>
-      <c r="C8" s="67"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
-      <c r="F8" s="69"/>
+      <c r="A8" s="62"/>
+      <c r="B8" s="63"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="70"/>
       <c r="G8" s="30"/>
       <c r="H8" s="30"/>
       <c r="I8" s="30"/>
-      <c r="J8" s="50"/>
-      <c r="K8" s="51"/>
-      <c r="L8" s="52"/>
-      <c r="M8" s="53"/>
-      <c r="N8" s="52"/>
-      <c r="O8" s="51"/>
+      <c r="J8" s="51"/>
+      <c r="K8" s="52"/>
+      <c r="L8" s="53"/>
+      <c r="M8" s="54"/>
+      <c r="N8" s="53"/>
+      <c r="O8" s="52"/>
     </row>
     <row r="9" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A9" s="20"/>
@@ -6832,7 +6842,7 @@
       <c r="G9" s="28"/>
       <c r="H9" s="28"/>
       <c r="I9" s="28"/>
-      <c r="J9" s="54"/>
+      <c r="J9" s="55"/>
       <c r="K9" s="23"/>
       <c r="L9" s="24"/>
       <c r="M9" s="22"/>
@@ -6849,7 +6859,7 @@
       <c r="G10" s="28"/>
       <c r="H10" s="28"/>
       <c r="I10" s="28"/>
-      <c r="J10" s="54"/>
+      <c r="J10" s="55"/>
       <c r="K10" s="23"/>
       <c r="L10" s="24"/>
       <c r="M10" s="22"/>
@@ -6866,7 +6876,7 @@
       <c r="G11" s="28"/>
       <c r="H11" s="28"/>
       <c r="I11" s="28"/>
-      <c r="J11" s="54"/>
+      <c r="J11" s="55"/>
       <c r="K11" s="23"/>
       <c r="L11" s="24"/>
       <c r="M11" s="22"/>
@@ -6883,7 +6893,7 @@
       <c r="G12" s="28"/>
       <c r="H12" s="28"/>
       <c r="I12" s="28"/>
-      <c r="J12" s="54"/>
+      <c r="J12" s="55"/>
       <c r="K12" s="23"/>
       <c r="L12" s="24"/>
       <c r="M12" s="22"/>
@@ -6900,7 +6910,7 @@
       <c r="G13" s="28"/>
       <c r="H13" s="28"/>
       <c r="I13" s="28"/>
-      <c r="J13" s="54"/>
+      <c r="J13" s="55"/>
       <c r="K13" s="23"/>
       <c r="L13" s="24"/>
       <c r="M13" s="22"/>
@@ -6917,7 +6927,7 @@
       <c r="G14" s="28"/>
       <c r="H14" s="28"/>
       <c r="I14" s="28"/>
-      <c r="J14" s="54"/>
+      <c r="J14" s="55"/>
       <c r="K14" s="23"/>
       <c r="L14" s="24"/>
       <c r="M14" s="22"/>
@@ -6934,7 +6944,7 @@
       <c r="G15" s="28"/>
       <c r="H15" s="28"/>
       <c r="I15" s="28"/>
-      <c r="J15" s="54"/>
+      <c r="J15" s="55"/>
       <c r="K15" s="23"/>
       <c r="L15" s="24"/>
       <c r="M15" s="22"/>
@@ -6943,7 +6953,7 @@
     </row>
     <row r="16" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A16" s="20"/>
-      <c r="B16" s="70"/>
+      <c r="B16" s="71"/>
       <c r="C16" s="27"/>
       <c r="D16" s="28"/>
       <c r="E16" s="28"/>
@@ -6951,7 +6961,7 @@
       <c r="G16" s="28"/>
       <c r="H16" s="28"/>
       <c r="I16" s="28"/>
-      <c r="J16" s="54"/>
+      <c r="J16" s="55"/>
       <c r="K16" s="23"/>
       <c r="L16" s="24"/>
       <c r="M16" s="22"/>
@@ -6968,7 +6978,7 @@
       <c r="G17" s="28"/>
       <c r="H17" s="28"/>
       <c r="I17" s="28"/>
-      <c r="J17" s="54"/>
+      <c r="J17" s="55"/>
       <c r="K17" s="23"/>
       <c r="L17" s="24"/>
       <c r="M17" s="22"/>
@@ -6985,7 +6995,7 @@
       <c r="G18" s="28"/>
       <c r="H18" s="28"/>
       <c r="I18" s="28"/>
-      <c r="J18" s="54"/>
+      <c r="J18" s="55"/>
       <c r="K18" s="23"/>
       <c r="L18" s="24"/>
       <c r="M18" s="22"/>
@@ -7002,7 +7012,7 @@
       <c r="G19" s="28"/>
       <c r="H19" s="28"/>
       <c r="I19" s="28"/>
-      <c r="J19" s="54"/>
+      <c r="J19" s="55"/>
       <c r="K19" s="23"/>
       <c r="L19" s="24"/>
       <c r="M19" s="22"/>
@@ -7019,7 +7029,7 @@
       <c r="G20" s="28"/>
       <c r="H20" s="28"/>
       <c r="I20" s="28"/>
-      <c r="J20" s="54"/>
+      <c r="J20" s="55"/>
       <c r="K20" s="23"/>
       <c r="L20" s="24"/>
       <c r="M20" s="22"/>
@@ -7036,7 +7046,7 @@
       <c r="G21" s="28"/>
       <c r="H21" s="28"/>
       <c r="I21" s="28"/>
-      <c r="J21" s="54"/>
+      <c r="J21" s="55"/>
       <c r="K21" s="23"/>
       <c r="L21" s="24"/>
       <c r="M21" s="22"/>
@@ -7053,7 +7063,7 @@
       <c r="G22" s="28"/>
       <c r="H22" s="28"/>
       <c r="I22" s="28"/>
-      <c r="J22" s="54"/>
+      <c r="J22" s="55"/>
       <c r="K22" s="23"/>
       <c r="L22" s="24"/>
       <c r="M22" s="22"/>
@@ -7070,7 +7080,7 @@
       <c r="G23" s="28"/>
       <c r="H23" s="28"/>
       <c r="I23" s="28"/>
-      <c r="J23" s="54"/>
+      <c r="J23" s="55"/>
       <c r="K23" s="23"/>
       <c r="L23" s="24"/>
       <c r="M23" s="22"/>
@@ -7087,7 +7097,7 @@
       <c r="G24" s="28"/>
       <c r="H24" s="28"/>
       <c r="I24" s="28"/>
-      <c r="J24" s="54"/>
+      <c r="J24" s="55"/>
       <c r="K24" s="23"/>
       <c r="L24" s="24"/>
       <c r="M24" s="22"/>
@@ -7104,7 +7114,7 @@
       <c r="G25" s="28"/>
       <c r="H25" s="28"/>
       <c r="I25" s="28"/>
-      <c r="J25" s="54"/>
+      <c r="J25" s="55"/>
       <c r="K25" s="23"/>
       <c r="L25" s="24"/>
       <c r="M25" s="22"/>
@@ -7121,7 +7131,7 @@
       <c r="G26" s="28"/>
       <c r="H26" s="28"/>
       <c r="I26" s="28"/>
-      <c r="J26" s="54"/>
+      <c r="J26" s="55"/>
       <c r="K26" s="23"/>
       <c r="L26" s="24"/>
       <c r="M26" s="22"/>
@@ -7138,7 +7148,7 @@
       <c r="G27" s="28"/>
       <c r="H27" s="28"/>
       <c r="I27" s="28"/>
-      <c r="J27" s="54"/>
+      <c r="J27" s="55"/>
       <c r="K27" s="23"/>
       <c r="L27" s="24"/>
       <c r="M27" s="22"/>
@@ -7155,7 +7165,7 @@
       <c r="G28" s="28"/>
       <c r="H28" s="28"/>
       <c r="I28" s="28"/>
-      <c r="J28" s="54"/>
+      <c r="J28" s="55"/>
       <c r="K28" s="23"/>
       <c r="L28" s="24"/>
       <c r="M28" s="22"/>
@@ -7172,7 +7182,7 @@
       <c r="G29" s="28"/>
       <c r="H29" s="28"/>
       <c r="I29" s="28"/>
-      <c r="J29" s="54"/>
+      <c r="J29" s="55"/>
       <c r="K29" s="23"/>
       <c r="L29" s="24"/>
       <c r="M29" s="22"/>
@@ -7189,7 +7199,7 @@
       <c r="G30" s="28"/>
       <c r="H30" s="28"/>
       <c r="I30" s="28"/>
-      <c r="J30" s="54"/>
+      <c r="J30" s="55"/>
       <c r="K30" s="23"/>
       <c r="L30" s="24"/>
       <c r="M30" s="22"/>
@@ -7206,7 +7216,7 @@
       <c r="G31" s="28"/>
       <c r="H31" s="28"/>
       <c r="I31" s="28"/>
-      <c r="J31" s="54"/>
+      <c r="J31" s="55"/>
       <c r="K31" s="23"/>
       <c r="L31" s="24"/>
       <c r="M31" s="22"/>
@@ -7223,7 +7233,7 @@
       <c r="G32" s="28"/>
       <c r="H32" s="28"/>
       <c r="I32" s="28"/>
-      <c r="J32" s="54"/>
+      <c r="J32" s="55"/>
       <c r="K32" s="23"/>
       <c r="L32" s="24"/>
       <c r="M32" s="22"/>
@@ -7240,7 +7250,7 @@
       <c r="G33" s="28"/>
       <c r="H33" s="28"/>
       <c r="I33" s="28"/>
-      <c r="J33" s="54"/>
+      <c r="J33" s="55"/>
       <c r="K33" s="23"/>
       <c r="L33" s="24"/>
       <c r="M33" s="22"/>
@@ -7257,7 +7267,7 @@
       <c r="G34" s="28"/>
       <c r="H34" s="28"/>
       <c r="I34" s="28"/>
-      <c r="J34" s="54"/>
+      <c r="J34" s="55"/>
       <c r="K34" s="23"/>
       <c r="L34" s="24"/>
       <c r="M34" s="22"/>
@@ -7274,7 +7284,7 @@
       <c r="G35" s="28"/>
       <c r="H35" s="28"/>
       <c r="I35" s="28"/>
-      <c r="J35" s="54"/>
+      <c r="J35" s="55"/>
       <c r="K35" s="23"/>
       <c r="L35" s="24"/>
       <c r="M35" s="22"/>
@@ -7291,7 +7301,7 @@
       <c r="G36" s="28"/>
       <c r="H36" s="28"/>
       <c r="I36" s="28"/>
-      <c r="J36" s="54"/>
+      <c r="J36" s="55"/>
       <c r="K36" s="23"/>
       <c r="L36" s="24"/>
       <c r="M36" s="22"/>
@@ -7308,7 +7318,7 @@
       <c r="G37" s="28"/>
       <c r="H37" s="28"/>
       <c r="I37" s="28"/>
-      <c r="J37" s="54"/>
+      <c r="J37" s="55"/>
       <c r="K37" s="23"/>
       <c r="L37" s="24"/>
       <c r="M37" s="22"/>
@@ -7325,7 +7335,7 @@
       <c r="G38" s="28"/>
       <c r="H38" s="28"/>
       <c r="I38" s="28"/>
-      <c r="J38" s="54"/>
+      <c r="J38" s="55"/>
       <c r="K38" s="23"/>
       <c r="L38" s="24"/>
       <c r="M38" s="22"/>
@@ -7342,7 +7352,7 @@
       <c r="G39" s="28"/>
       <c r="H39" s="28"/>
       <c r="I39" s="28"/>
-      <c r="J39" s="54"/>
+      <c r="J39" s="55"/>
       <c r="K39" s="23"/>
       <c r="L39" s="24"/>
       <c r="M39" s="22"/>
@@ -7359,7 +7369,7 @@
       <c r="G40" s="28"/>
       <c r="H40" s="28"/>
       <c r="I40" s="28"/>
-      <c r="J40" s="54"/>
+      <c r="J40" s="55"/>
       <c r="K40" s="23"/>
       <c r="L40" s="24"/>
       <c r="M40" s="22"/>
@@ -7376,7 +7386,7 @@
       <c r="G41" s="28"/>
       <c r="H41" s="28"/>
       <c r="I41" s="28"/>
-      <c r="J41" s="54"/>
+      <c r="J41" s="55"/>
       <c r="K41" s="23"/>
       <c r="L41" s="24"/>
       <c r="M41" s="22"/>
@@ -7393,7 +7403,7 @@
       <c r="G42" s="28"/>
       <c r="H42" s="28"/>
       <c r="I42" s="28"/>
-      <c r="J42" s="54"/>
+      <c r="J42" s="55"/>
       <c r="K42" s="23"/>
       <c r="L42" s="24"/>
       <c r="M42" s="22"/>
@@ -7410,7 +7420,7 @@
       <c r="G43" s="28"/>
       <c r="H43" s="28"/>
       <c r="I43" s="28"/>
-      <c r="J43" s="54"/>
+      <c r="J43" s="55"/>
       <c r="K43" s="23"/>
       <c r="L43" s="24"/>
       <c r="M43" s="22"/>
@@ -7427,7 +7437,7 @@
       <c r="G44" s="28"/>
       <c r="H44" s="28"/>
       <c r="I44" s="28"/>
-      <c r="J44" s="54"/>
+      <c r="J44" s="55"/>
       <c r="K44" s="23"/>
       <c r="L44" s="24"/>
       <c r="M44" s="22"/>
@@ -7444,7 +7454,7 @@
       <c r="G45" s="28"/>
       <c r="H45" s="28"/>
       <c r="I45" s="28"/>
-      <c r="J45" s="54"/>
+      <c r="J45" s="55"/>
       <c r="K45" s="23"/>
       <c r="L45" s="24"/>
       <c r="M45" s="22"/>
@@ -7461,7 +7471,7 @@
       <c r="G46" s="28"/>
       <c r="H46" s="28"/>
       <c r="I46" s="28"/>
-      <c r="J46" s="54"/>
+      <c r="J46" s="55"/>
       <c r="K46" s="23"/>
       <c r="L46" s="24"/>
       <c r="M46" s="22"/>
@@ -7478,7 +7488,7 @@
       <c r="G47" s="28"/>
       <c r="H47" s="28"/>
       <c r="I47" s="28"/>
-      <c r="J47" s="54"/>
+      <c r="J47" s="55"/>
       <c r="K47" s="23"/>
       <c r="L47" s="24"/>
       <c r="M47" s="22"/>
@@ -7495,7 +7505,7 @@
       <c r="G48" s="28"/>
       <c r="H48" s="28"/>
       <c r="I48" s="28"/>
-      <c r="J48" s="54"/>
+      <c r="J48" s="55"/>
       <c r="K48" s="23"/>
       <c r="L48" s="24"/>
       <c r="M48" s="22"/>
@@ -7512,7 +7522,7 @@
       <c r="G49" s="28"/>
       <c r="H49" s="28"/>
       <c r="I49" s="28"/>
-      <c r="J49" s="54"/>
+      <c r="J49" s="55"/>
       <c r="K49" s="23"/>
       <c r="L49" s="24"/>
       <c r="M49" s="22"/>
@@ -7529,7 +7539,7 @@
       <c r="G50" s="28"/>
       <c r="H50" s="28"/>
       <c r="I50" s="28"/>
-      <c r="J50" s="54"/>
+      <c r="J50" s="55"/>
       <c r="K50" s="23"/>
       <c r="L50" s="24"/>
       <c r="M50" s="22"/>
@@ -7546,7 +7556,7 @@
       <c r="G51" s="28"/>
       <c r="H51" s="28"/>
       <c r="I51" s="28"/>
-      <c r="J51" s="54"/>
+      <c r="J51" s="55"/>
       <c r="K51" s="23"/>
       <c r="L51" s="24"/>
       <c r="M51" s="22"/>
@@ -7563,7 +7573,7 @@
       <c r="G52" s="28"/>
       <c r="H52" s="28"/>
       <c r="I52" s="28"/>
-      <c r="J52" s="54"/>
+      <c r="J52" s="55"/>
       <c r="K52" s="23"/>
       <c r="L52" s="24"/>
       <c r="M52" s="22"/>
@@ -7580,7 +7590,7 @@
       <c r="G53" s="28"/>
       <c r="H53" s="28"/>
       <c r="I53" s="28"/>
-      <c r="J53" s="54"/>
+      <c r="J53" s="55"/>
       <c r="K53" s="23"/>
       <c r="L53" s="24"/>
       <c r="M53" s="22"/>
@@ -7597,7 +7607,7 @@
       <c r="G54" s="28"/>
       <c r="H54" s="28"/>
       <c r="I54" s="28"/>
-      <c r="J54" s="54"/>
+      <c r="J54" s="55"/>
       <c r="K54" s="23"/>
       <c r="L54" s="24"/>
       <c r="M54" s="22"/>
@@ -7614,7 +7624,7 @@
       <c r="G55" s="28"/>
       <c r="H55" s="28"/>
       <c r="I55" s="28"/>
-      <c r="J55" s="54"/>
+      <c r="J55" s="55"/>
       <c r="K55" s="23"/>
       <c r="L55" s="24"/>
       <c r="M55" s="22"/>
@@ -7631,7 +7641,7 @@
       <c r="G56" s="28"/>
       <c r="H56" s="28"/>
       <c r="I56" s="28"/>
-      <c r="J56" s="54"/>
+      <c r="J56" s="55"/>
       <c r="K56" s="23"/>
       <c r="L56" s="24"/>
       <c r="M56" s="22"/>
@@ -7648,7 +7658,7 @@
       <c r="G57" s="28"/>
       <c r="H57" s="28"/>
       <c r="I57" s="28"/>
-      <c r="J57" s="54"/>
+      <c r="J57" s="55"/>
       <c r="K57" s="23"/>
       <c r="L57" s="24"/>
       <c r="M57" s="22"/>
@@ -7665,7 +7675,7 @@
       <c r="G58" s="28"/>
       <c r="H58" s="28"/>
       <c r="I58" s="28"/>
-      <c r="J58" s="54"/>
+      <c r="J58" s="55"/>
       <c r="K58" s="23"/>
       <c r="L58" s="24"/>
       <c r="M58" s="22"/>
@@ -7682,7 +7692,7 @@
       <c r="G59" s="28"/>
       <c r="H59" s="28"/>
       <c r="I59" s="28"/>
-      <c r="J59" s="54"/>
+      <c r="J59" s="55"/>
       <c r="K59" s="23"/>
       <c r="L59" s="24"/>
       <c r="M59" s="22"/>
@@ -7699,7 +7709,7 @@
       <c r="G60" s="28"/>
       <c r="H60" s="28"/>
       <c r="I60" s="28"/>
-      <c r="J60" s="54"/>
+      <c r="J60" s="55"/>
       <c r="K60" s="23"/>
       <c r="L60" s="24"/>
       <c r="M60" s="22"/>
@@ -7716,7 +7726,7 @@
       <c r="G61" s="28"/>
       <c r="H61" s="28"/>
       <c r="I61" s="28"/>
-      <c r="J61" s="54"/>
+      <c r="J61" s="55"/>
       <c r="K61" s="23"/>
       <c r="L61" s="24"/>
       <c r="M61" s="22"/>
@@ -7733,7 +7743,7 @@
       <c r="G62" s="28"/>
       <c r="H62" s="28"/>
       <c r="I62" s="28"/>
-      <c r="J62" s="54"/>
+      <c r="J62" s="55"/>
       <c r="K62" s="23"/>
       <c r="L62" s="24"/>
       <c r="M62" s="22"/>
@@ -7750,7 +7760,7 @@
       <c r="G63" s="28"/>
       <c r="H63" s="28"/>
       <c r="I63" s="28"/>
-      <c r="J63" s="54"/>
+      <c r="J63" s="55"/>
       <c r="K63" s="23"/>
       <c r="L63" s="24"/>
       <c r="M63" s="22"/>
@@ -7767,7 +7777,7 @@
       <c r="G64" s="28"/>
       <c r="H64" s="28"/>
       <c r="I64" s="28"/>
-      <c r="J64" s="54"/>
+      <c r="J64" s="55"/>
       <c r="K64" s="23"/>
       <c r="L64" s="24"/>
       <c r="M64" s="22"/>
@@ -7784,7 +7794,7 @@
       <c r="G65" s="28"/>
       <c r="H65" s="28"/>
       <c r="I65" s="28"/>
-      <c r="J65" s="54"/>
+      <c r="J65" s="55"/>
       <c r="K65" s="23"/>
       <c r="L65" s="24"/>
       <c r="M65" s="22"/>
@@ -7801,7 +7811,7 @@
       <c r="G66" s="28"/>
       <c r="H66" s="28"/>
       <c r="I66" s="28"/>
-      <c r="J66" s="54"/>
+      <c r="J66" s="55"/>
       <c r="K66" s="23"/>
       <c r="L66" s="24"/>
       <c r="M66" s="22"/>
@@ -7818,7 +7828,7 @@
       <c r="G67" s="28"/>
       <c r="H67" s="28"/>
       <c r="I67" s="28"/>
-      <c r="J67" s="54"/>
+      <c r="J67" s="55"/>
       <c r="K67" s="23"/>
       <c r="L67" s="24"/>
       <c r="M67" s="22"/>
@@ -7835,7 +7845,7 @@
       <c r="G68" s="28"/>
       <c r="H68" s="28"/>
       <c r="I68" s="28"/>
-      <c r="J68" s="54"/>
+      <c r="J68" s="55"/>
       <c r="K68" s="23"/>
       <c r="L68" s="24"/>
       <c r="M68" s="22"/>
@@ -7852,7 +7862,7 @@
       <c r="G69" s="28"/>
       <c r="H69" s="28"/>
       <c r="I69" s="28"/>
-      <c r="J69" s="54"/>
+      <c r="J69" s="55"/>
       <c r="K69" s="23"/>
       <c r="L69" s="24"/>
       <c r="M69" s="22"/>
@@ -7869,7 +7879,7 @@
       <c r="G70" s="28"/>
       <c r="H70" s="28"/>
       <c r="I70" s="28"/>
-      <c r="J70" s="54"/>
+      <c r="J70" s="55"/>
       <c r="K70" s="23"/>
       <c r="L70" s="24"/>
       <c r="M70" s="22"/>
@@ -7886,7 +7896,7 @@
       <c r="G71" s="28"/>
       <c r="H71" s="28"/>
       <c r="I71" s="28"/>
-      <c r="J71" s="54"/>
+      <c r="J71" s="55"/>
       <c r="K71" s="23"/>
       <c r="L71" s="24"/>
       <c r="M71" s="22"/>
@@ -7903,7 +7913,7 @@
       <c r="G72" s="28"/>
       <c r="H72" s="28"/>
       <c r="I72" s="28"/>
-      <c r="J72" s="54"/>
+      <c r="J72" s="55"/>
       <c r="K72" s="23"/>
       <c r="L72" s="24"/>
       <c r="M72" s="22"/>
@@ -7920,7 +7930,7 @@
       <c r="G73" s="28"/>
       <c r="H73" s="28"/>
       <c r="I73" s="28"/>
-      <c r="J73" s="54"/>
+      <c r="J73" s="55"/>
       <c r="K73" s="23"/>
       <c r="L73" s="24"/>
       <c r="M73" s="22"/>
@@ -7937,7 +7947,7 @@
       <c r="G74" s="28"/>
       <c r="H74" s="28"/>
       <c r="I74" s="28"/>
-      <c r="J74" s="54"/>
+      <c r="J74" s="55"/>
       <c r="K74" s="23"/>
       <c r="L74" s="24"/>
       <c r="M74" s="22"/>
@@ -7954,7 +7964,7 @@
       <c r="G75" s="28"/>
       <c r="H75" s="28"/>
       <c r="I75" s="28"/>
-      <c r="J75" s="54"/>
+      <c r="J75" s="55"/>
       <c r="K75" s="23"/>
       <c r="L75" s="24"/>
       <c r="M75" s="22"/>
@@ -7971,7 +7981,7 @@
       <c r="G76" s="28"/>
       <c r="H76" s="28"/>
       <c r="I76" s="28"/>
-      <c r="J76" s="54"/>
+      <c r="J76" s="55"/>
       <c r="K76" s="23"/>
       <c r="L76" s="24"/>
       <c r="M76" s="22"/>
@@ -7988,7 +7998,7 @@
       <c r="G77" s="28"/>
       <c r="H77" s="28"/>
       <c r="I77" s="28"/>
-      <c r="J77" s="54"/>
+      <c r="J77" s="55"/>
       <c r="K77" s="23"/>
       <c r="L77" s="24"/>
       <c r="M77" s="22"/>
@@ -8005,7 +8015,7 @@
       <c r="G78" s="28"/>
       <c r="H78" s="28"/>
       <c r="I78" s="28"/>
-      <c r="J78" s="54"/>
+      <c r="J78" s="55"/>
       <c r="K78" s="23"/>
       <c r="L78" s="24"/>
       <c r="M78" s="22"/>
@@ -8022,7 +8032,7 @@
       <c r="G79" s="28"/>
       <c r="H79" s="28"/>
       <c r="I79" s="28"/>
-      <c r="J79" s="54"/>
+      <c r="J79" s="55"/>
       <c r="K79" s="23"/>
       <c r="L79" s="24"/>
       <c r="M79" s="22"/>
@@ -8039,7 +8049,7 @@
       <c r="G80" s="28"/>
       <c r="H80" s="28"/>
       <c r="I80" s="28"/>
-      <c r="J80" s="54"/>
+      <c r="J80" s="55"/>
       <c r="K80" s="23"/>
       <c r="L80" s="24"/>
       <c r="M80" s="22"/>
@@ -8056,7 +8066,7 @@
       <c r="G81" s="28"/>
       <c r="H81" s="28"/>
       <c r="I81" s="28"/>
-      <c r="J81" s="54"/>
+      <c r="J81" s="55"/>
       <c r="K81" s="23"/>
       <c r="L81" s="24"/>
       <c r="M81" s="22"/>
@@ -8073,7 +8083,7 @@
       <c r="G82" s="28"/>
       <c r="H82" s="28"/>
       <c r="I82" s="28"/>
-      <c r="J82" s="54"/>
+      <c r="J82" s="55"/>
       <c r="K82" s="23"/>
       <c r="L82" s="24"/>
       <c r="M82" s="22"/>
@@ -8090,7 +8100,7 @@
       <c r="G83" s="28"/>
       <c r="H83" s="28"/>
       <c r="I83" s="28"/>
-      <c r="J83" s="54"/>
+      <c r="J83" s="55"/>
       <c r="K83" s="23"/>
       <c r="L83" s="24"/>
       <c r="M83" s="22"/>
@@ -8107,7 +8117,7 @@
       <c r="G84" s="28"/>
       <c r="H84" s="28"/>
       <c r="I84" s="28"/>
-      <c r="J84" s="54"/>
+      <c r="J84" s="55"/>
       <c r="K84" s="23"/>
       <c r="L84" s="24"/>
       <c r="M84" s="22"/>
@@ -8124,7 +8134,7 @@
       <c r="G85" s="28"/>
       <c r="H85" s="28"/>
       <c r="I85" s="28"/>
-      <c r="J85" s="54"/>
+      <c r="J85" s="55"/>
       <c r="K85" s="23"/>
       <c r="L85" s="24"/>
       <c r="M85" s="22"/>
@@ -8141,7 +8151,7 @@
       <c r="G86" s="28"/>
       <c r="H86" s="28"/>
       <c r="I86" s="28"/>
-      <c r="J86" s="54"/>
+      <c r="J86" s="55"/>
       <c r="K86" s="23"/>
       <c r="L86" s="24"/>
       <c r="M86" s="22"/>
@@ -8158,7 +8168,7 @@
       <c r="G87" s="28"/>
       <c r="H87" s="28"/>
       <c r="I87" s="28"/>
-      <c r="J87" s="54"/>
+      <c r="J87" s="55"/>
       <c r="K87" s="23"/>
       <c r="L87" s="24"/>
       <c r="M87" s="22"/>
@@ -8175,7 +8185,7 @@
       <c r="G88" s="28"/>
       <c r="H88" s="28"/>
       <c r="I88" s="28"/>
-      <c r="J88" s="54"/>
+      <c r="J88" s="55"/>
       <c r="K88" s="23"/>
       <c r="L88" s="24"/>
       <c r="M88" s="22"/>
@@ -8192,7 +8202,7 @@
       <c r="G89" s="28"/>
       <c r="H89" s="28"/>
       <c r="I89" s="28"/>
-      <c r="J89" s="54"/>
+      <c r="J89" s="55"/>
       <c r="K89" s="23"/>
       <c r="L89" s="24"/>
       <c r="M89" s="22"/>
@@ -8209,7 +8219,7 @@
       <c r="G90" s="28"/>
       <c r="H90" s="28"/>
       <c r="I90" s="28"/>
-      <c r="J90" s="54"/>
+      <c r="J90" s="55"/>
       <c r="K90" s="23"/>
       <c r="L90" s="24"/>
       <c r="M90" s="22"/>
@@ -8226,7 +8236,7 @@
       <c r="G91" s="28"/>
       <c r="H91" s="28"/>
       <c r="I91" s="28"/>
-      <c r="J91" s="54"/>
+      <c r="J91" s="55"/>
       <c r="K91" s="23"/>
       <c r="L91" s="24"/>
       <c r="M91" s="22"/>
@@ -8243,7 +8253,7 @@
       <c r="G92" s="28"/>
       <c r="H92" s="28"/>
       <c r="I92" s="28"/>
-      <c r="J92" s="54"/>
+      <c r="J92" s="55"/>
       <c r="K92" s="23"/>
       <c r="L92" s="24"/>
       <c r="M92" s="22"/>
@@ -8260,7 +8270,7 @@
       <c r="G93" s="28"/>
       <c r="H93" s="28"/>
       <c r="I93" s="28"/>
-      <c r="J93" s="54"/>
+      <c r="J93" s="55"/>
       <c r="K93" s="23"/>
       <c r="L93" s="24"/>
       <c r="M93" s="22"/>
@@ -8277,7 +8287,7 @@
       <c r="G94" s="28"/>
       <c r="H94" s="28"/>
       <c r="I94" s="28"/>
-      <c r="J94" s="54"/>
+      <c r="J94" s="55"/>
       <c r="K94" s="23"/>
       <c r="L94" s="24"/>
       <c r="M94" s="22"/>
@@ -8294,7 +8304,7 @@
       <c r="G95" s="28"/>
       <c r="H95" s="28"/>
       <c r="I95" s="28"/>
-      <c r="J95" s="54"/>
+      <c r="J95" s="55"/>
       <c r="K95" s="23"/>
       <c r="L95" s="24"/>
       <c r="M95" s="22"/>
@@ -8311,7 +8321,7 @@
       <c r="G96" s="28"/>
       <c r="H96" s="28"/>
       <c r="I96" s="28"/>
-      <c r="J96" s="54"/>
+      <c r="J96" s="55"/>
       <c r="K96" s="23"/>
       <c r="L96" s="24"/>
       <c r="M96" s="22"/>
@@ -8328,7 +8338,7 @@
       <c r="G97" s="28"/>
       <c r="H97" s="28"/>
       <c r="I97" s="28"/>
-      <c r="J97" s="54"/>
+      <c r="J97" s="55"/>
       <c r="K97" s="23"/>
       <c r="L97" s="24"/>
       <c r="M97" s="22"/>
@@ -8345,7 +8355,7 @@
       <c r="G98" s="28"/>
       <c r="H98" s="28"/>
       <c r="I98" s="28"/>
-      <c r="J98" s="54"/>
+      <c r="J98" s="55"/>
       <c r="K98" s="23"/>
       <c r="L98" s="24"/>
       <c r="M98" s="22"/>
@@ -8362,7 +8372,7 @@
       <c r="G99" s="28"/>
       <c r="H99" s="28"/>
       <c r="I99" s="28"/>
-      <c r="J99" s="54"/>
+      <c r="J99" s="55"/>
       <c r="K99" s="23"/>
       <c r="L99" s="24"/>
       <c r="M99" s="22"/>
@@ -8379,7 +8389,7 @@
       <c r="G100" s="28"/>
       <c r="H100" s="28"/>
       <c r="I100" s="28"/>
-      <c r="J100" s="54"/>
+      <c r="J100" s="55"/>
       <c r="K100" s="23"/>
       <c r="L100" s="24"/>
       <c r="M100" s="22"/>
@@ -8396,7 +8406,7 @@
       <c r="G101" s="28"/>
       <c r="H101" s="28"/>
       <c r="I101" s="28"/>
-      <c r="J101" s="54"/>
+      <c r="J101" s="55"/>
       <c r="K101" s="23"/>
       <c r="L101" s="24"/>
       <c r="M101" s="22"/>
@@ -8413,7 +8423,7 @@
       <c r="G102" s="28"/>
       <c r="H102" s="28"/>
       <c r="I102" s="28"/>
-      <c r="J102" s="54"/>
+      <c r="J102" s="55"/>
       <c r="K102" s="23"/>
       <c r="L102" s="24"/>
       <c r="M102" s="22"/>
@@ -8430,7 +8440,7 @@
       <c r="G103" s="28"/>
       <c r="H103" s="28"/>
       <c r="I103" s="28"/>
-      <c r="J103" s="54"/>
+      <c r="J103" s="55"/>
       <c r="K103" s="23"/>
       <c r="L103" s="24"/>
       <c r="M103" s="22"/>
@@ -8447,7 +8457,7 @@
       <c r="G104" s="28"/>
       <c r="H104" s="28"/>
       <c r="I104" s="28"/>
-      <c r="J104" s="54"/>
+      <c r="J104" s="55"/>
       <c r="K104" s="23"/>
       <c r="L104" s="24"/>
       <c r="M104" s="22"/>
@@ -8464,7 +8474,7 @@
       <c r="G105" s="28"/>
       <c r="H105" s="28"/>
       <c r="I105" s="28"/>
-      <c r="J105" s="54"/>
+      <c r="J105" s="55"/>
       <c r="K105" s="23"/>
       <c r="L105" s="24"/>
       <c r="M105" s="22"/>
@@ -8481,7 +8491,7 @@
       <c r="G106" s="28"/>
       <c r="H106" s="28"/>
       <c r="I106" s="28"/>
-      <c r="J106" s="54"/>
+      <c r="J106" s="55"/>
       <c r="K106" s="23"/>
       <c r="L106" s="24"/>
       <c r="M106" s="22"/>
@@ -8498,7 +8508,7 @@
       <c r="G107" s="28"/>
       <c r="H107" s="28"/>
       <c r="I107" s="28"/>
-      <c r="J107" s="54"/>
+      <c r="J107" s="55"/>
       <c r="K107" s="23"/>
       <c r="L107" s="24"/>
       <c r="M107" s="22"/>
@@ -8515,7 +8525,7 @@
       <c r="G108" s="28"/>
       <c r="H108" s="28"/>
       <c r="I108" s="28"/>
-      <c r="J108" s="54"/>
+      <c r="J108" s="55"/>
       <c r="K108" s="23"/>
       <c r="L108" s="24"/>
       <c r="M108" s="22"/>
@@ -8532,7 +8542,7 @@
       <c r="G109" s="28"/>
       <c r="H109" s="28"/>
       <c r="I109" s="28"/>
-      <c r="J109" s="54"/>
+      <c r="J109" s="55"/>
       <c r="K109" s="23"/>
       <c r="L109" s="24"/>
       <c r="M109" s="22"/>
@@ -8549,7 +8559,7 @@
       <c r="G110" s="28"/>
       <c r="H110" s="28"/>
       <c r="I110" s="28"/>
-      <c r="J110" s="54"/>
+      <c r="J110" s="55"/>
       <c r="K110" s="23"/>
       <c r="L110" s="24"/>
       <c r="M110" s="22"/>
@@ -8566,7 +8576,7 @@
       <c r="G111" s="28"/>
       <c r="H111" s="28"/>
       <c r="I111" s="28"/>
-      <c r="J111" s="54"/>
+      <c r="J111" s="55"/>
       <c r="K111" s="23"/>
       <c r="L111" s="24"/>
       <c r="M111" s="22"/>
@@ -8583,7 +8593,7 @@
       <c r="G112" s="28"/>
       <c r="H112" s="28"/>
       <c r="I112" s="28"/>
-      <c r="J112" s="54"/>
+      <c r="J112" s="55"/>
       <c r="K112" s="23"/>
       <c r="L112" s="24"/>
       <c r="M112" s="22"/>
@@ -8600,7 +8610,7 @@
       <c r="G113" s="28"/>
       <c r="H113" s="28"/>
       <c r="I113" s="28"/>
-      <c r="J113" s="54"/>
+      <c r="J113" s="55"/>
       <c r="K113" s="23"/>
       <c r="L113" s="24"/>
       <c r="M113" s="22"/>
@@ -8617,7 +8627,7 @@
       <c r="G114" s="28"/>
       <c r="H114" s="28"/>
       <c r="I114" s="28"/>
-      <c r="J114" s="54"/>
+      <c r="J114" s="55"/>
       <c r="K114" s="23"/>
       <c r="L114" s="24"/>
       <c r="M114" s="22"/>
@@ -8634,7 +8644,7 @@
       <c r="G115" s="28"/>
       <c r="H115" s="28"/>
       <c r="I115" s="28"/>
-      <c r="J115" s="54"/>
+      <c r="J115" s="55"/>
       <c r="K115" s="23"/>
       <c r="L115" s="24"/>
       <c r="M115" s="22"/>
@@ -8651,7 +8661,7 @@
       <c r="G116" s="28"/>
       <c r="H116" s="28"/>
       <c r="I116" s="28"/>
-      <c r="J116" s="54"/>
+      <c r="J116" s="55"/>
       <c r="K116" s="23"/>
       <c r="L116" s="24"/>
       <c r="M116" s="22"/>
@@ -8668,7 +8678,7 @@
       <c r="G117" s="28"/>
       <c r="H117" s="28"/>
       <c r="I117" s="28"/>
-      <c r="J117" s="54"/>
+      <c r="J117" s="55"/>
       <c r="K117" s="23"/>
       <c r="L117" s="24"/>
       <c r="M117" s="22"/>
@@ -8685,7 +8695,7 @@
       <c r="G118" s="28"/>
       <c r="H118" s="28"/>
       <c r="I118" s="28"/>
-      <c r="J118" s="54"/>
+      <c r="J118" s="55"/>
       <c r="K118" s="23"/>
       <c r="L118" s="24"/>
       <c r="M118" s="22"/>
@@ -8702,7 +8712,7 @@
       <c r="G119" s="28"/>
       <c r="H119" s="28"/>
       <c r="I119" s="28"/>
-      <c r="J119" s="54"/>
+      <c r="J119" s="55"/>
       <c r="K119" s="23"/>
       <c r="L119" s="24"/>
       <c r="M119" s="22"/>
@@ -8719,7 +8729,7 @@
       <c r="G120" s="28"/>
       <c r="H120" s="28"/>
       <c r="I120" s="28"/>
-      <c r="J120" s="54"/>
+      <c r="J120" s="55"/>
       <c r="K120" s="23"/>
       <c r="L120" s="24"/>
       <c r="M120" s="22"/>
@@ -8736,7 +8746,7 @@
       <c r="G121" s="28"/>
       <c r="H121" s="28"/>
       <c r="I121" s="28"/>
-      <c r="J121" s="54"/>
+      <c r="J121" s="55"/>
       <c r="K121" s="23"/>
       <c r="L121" s="24"/>
       <c r="M121" s="22"/>
@@ -8753,7 +8763,7 @@
       <c r="G122" s="28"/>
       <c r="H122" s="28"/>
       <c r="I122" s="28"/>
-      <c r="J122" s="54"/>
+      <c r="J122" s="55"/>
       <c r="K122" s="23"/>
       <c r="L122" s="24"/>
       <c r="M122" s="22"/>
@@ -8770,7 +8780,7 @@
       <c r="G123" s="28"/>
       <c r="H123" s="28"/>
       <c r="I123" s="28"/>
-      <c r="J123" s="54"/>
+      <c r="J123" s="55"/>
       <c r="K123" s="23"/>
       <c r="L123" s="24"/>
       <c r="M123" s="22"/>
@@ -8787,7 +8797,7 @@
       <c r="G124" s="28"/>
       <c r="H124" s="28"/>
       <c r="I124" s="28"/>
-      <c r="J124" s="54"/>
+      <c r="J124" s="55"/>
       <c r="K124" s="23"/>
       <c r="L124" s="24"/>
       <c r="M124" s="22"/>
@@ -8804,7 +8814,7 @@
       <c r="G125" s="28"/>
       <c r="H125" s="28"/>
       <c r="I125" s="28"/>
-      <c r="J125" s="54"/>
+      <c r="J125" s="55"/>
       <c r="K125" s="23"/>
       <c r="L125" s="24"/>
       <c r="M125" s="22"/>
@@ -8821,7 +8831,7 @@
       <c r="G126" s="28"/>
       <c r="H126" s="28"/>
       <c r="I126" s="28"/>
-      <c r="J126" s="54"/>
+      <c r="J126" s="55"/>
       <c r="K126" s="23"/>
       <c r="L126" s="24"/>
       <c r="M126" s="22"/>
@@ -8838,7 +8848,7 @@
       <c r="G127" s="28"/>
       <c r="H127" s="28"/>
       <c r="I127" s="28"/>
-      <c r="J127" s="54"/>
+      <c r="J127" s="55"/>
       <c r="K127" s="23"/>
       <c r="L127" s="24"/>
       <c r="M127" s="22"/>
@@ -8855,7 +8865,7 @@
       <c r="G128" s="28"/>
       <c r="H128" s="28"/>
       <c r="I128" s="28"/>
-      <c r="J128" s="54"/>
+      <c r="J128" s="55"/>
       <c r="K128" s="23"/>
       <c r="L128" s="24"/>
       <c r="M128" s="22"/>
@@ -8872,7 +8882,7 @@
       <c r="G129" s="28"/>
       <c r="H129" s="28"/>
       <c r="I129" s="28"/>
-      <c r="J129" s="54"/>
+      <c r="J129" s="55"/>
       <c r="K129" s="23"/>
       <c r="L129" s="24"/>
       <c r="M129" s="22"/>
@@ -8889,7 +8899,7 @@
       <c r="G130" s="28"/>
       <c r="H130" s="28"/>
       <c r="I130" s="28"/>
-      <c r="J130" s="54"/>
+      <c r="J130" s="55"/>
       <c r="K130" s="23"/>
       <c r="L130" s="24"/>
       <c r="M130" s="22"/>
@@ -8906,7 +8916,7 @@
       <c r="G131" s="28"/>
       <c r="H131" s="28"/>
       <c r="I131" s="28"/>
-      <c r="J131" s="54"/>
+      <c r="J131" s="55"/>
       <c r="K131" s="23"/>
       <c r="L131" s="24"/>
       <c r="M131" s="22"/>
@@ -8923,7 +8933,7 @@
       <c r="G132" s="28"/>
       <c r="H132" s="28"/>
       <c r="I132" s="28"/>
-      <c r="J132" s="54"/>
+      <c r="J132" s="55"/>
       <c r="K132" s="23"/>
       <c r="L132" s="24"/>
       <c r="M132" s="22"/>
@@ -8940,7 +8950,7 @@
       <c r="G133" s="28"/>
       <c r="H133" s="28"/>
       <c r="I133" s="28"/>
-      <c r="J133" s="54"/>
+      <c r="J133" s="55"/>
       <c r="K133" s="23"/>
       <c r="L133" s="24"/>
       <c r="M133" s="22"/>
@@ -8957,7 +8967,7 @@
       <c r="G134" s="28"/>
       <c r="H134" s="28"/>
       <c r="I134" s="28"/>
-      <c r="J134" s="54"/>
+      <c r="J134" s="55"/>
       <c r="K134" s="23"/>
       <c r="L134" s="24"/>
       <c r="M134" s="22"/>
@@ -8974,7 +8984,7 @@
       <c r="G135" s="28"/>
       <c r="H135" s="28"/>
       <c r="I135" s="28"/>
-      <c r="J135" s="54"/>
+      <c r="J135" s="55"/>
       <c r="K135" s="23"/>
       <c r="L135" s="24"/>
       <c r="M135" s="22"/>
@@ -8991,7 +9001,7 @@
       <c r="G136" s="28"/>
       <c r="H136" s="28"/>
       <c r="I136" s="28"/>
-      <c r="J136" s="54"/>
+      <c r="J136" s="55"/>
       <c r="K136" s="23"/>
       <c r="L136" s="24"/>
       <c r="M136" s="22"/>
@@ -9008,7 +9018,7 @@
       <c r="G137" s="28"/>
       <c r="H137" s="28"/>
       <c r="I137" s="28"/>
-      <c r="J137" s="54"/>
+      <c r="J137" s="55"/>
       <c r="K137" s="23"/>
       <c r="L137" s="24"/>
       <c r="M137" s="22"/>
@@ -9025,7 +9035,7 @@
       <c r="G138" s="28"/>
       <c r="H138" s="28"/>
       <c r="I138" s="28"/>
-      <c r="J138" s="54"/>
+      <c r="J138" s="55"/>
       <c r="K138" s="23"/>
       <c r="L138" s="24"/>
       <c r="M138" s="22"/>
@@ -9042,7 +9052,7 @@
       <c r="G139" s="28"/>
       <c r="H139" s="28"/>
       <c r="I139" s="28"/>
-      <c r="J139" s="54"/>
+      <c r="J139" s="55"/>
       <c r="K139" s="23"/>
       <c r="L139" s="24"/>
       <c r="M139" s="22"/>
@@ -9059,7 +9069,7 @@
       <c r="G140" s="28"/>
       <c r="H140" s="28"/>
       <c r="I140" s="28"/>
-      <c r="J140" s="54"/>
+      <c r="J140" s="55"/>
       <c r="K140" s="23"/>
       <c r="L140" s="24"/>
       <c r="M140" s="22"/>
@@ -9076,7 +9086,7 @@
       <c r="G141" s="28"/>
       <c r="H141" s="28"/>
       <c r="I141" s="28"/>
-      <c r="J141" s="54"/>
+      <c r="J141" s="55"/>
       <c r="K141" s="23"/>
       <c r="L141" s="24"/>
       <c r="M141" s="22"/>
@@ -9093,7 +9103,7 @@
       <c r="G142" s="28"/>
       <c r="H142" s="28"/>
       <c r="I142" s="28"/>
-      <c r="J142" s="54"/>
+      <c r="J142" s="55"/>
       <c r="K142" s="23"/>
       <c r="L142" s="24"/>
       <c r="M142" s="22"/>
@@ -9110,7 +9120,7 @@
       <c r="G143" s="28"/>
       <c r="H143" s="28"/>
       <c r="I143" s="28"/>
-      <c r="J143" s="54"/>
+      <c r="J143" s="55"/>
       <c r="K143" s="23"/>
       <c r="L143" s="24"/>
       <c r="M143" s="22"/>
@@ -9127,7 +9137,7 @@
       <c r="G144" s="28"/>
       <c r="H144" s="28"/>
       <c r="I144" s="28"/>
-      <c r="J144" s="54"/>
+      <c r="J144" s="55"/>
       <c r="K144" s="23"/>
       <c r="L144" s="24"/>
       <c r="M144" s="22"/>
@@ -9144,7 +9154,7 @@
       <c r="G145" s="28"/>
       <c r="H145" s="28"/>
       <c r="I145" s="28"/>
-      <c r="J145" s="54"/>
+      <c r="J145" s="55"/>
       <c r="K145" s="23"/>
       <c r="L145" s="24"/>
       <c r="M145" s="22"/>
@@ -9161,7 +9171,7 @@
       <c r="G146" s="28"/>
       <c r="H146" s="28"/>
       <c r="I146" s="28"/>
-      <c r="J146" s="54"/>
+      <c r="J146" s="55"/>
       <c r="K146" s="23"/>
       <c r="L146" s="24"/>
       <c r="M146" s="22"/>
@@ -9178,7 +9188,7 @@
       <c r="G147" s="28"/>
       <c r="H147" s="28"/>
       <c r="I147" s="28"/>
-      <c r="J147" s="54"/>
+      <c r="J147" s="55"/>
       <c r="K147" s="23"/>
       <c r="L147" s="24"/>
       <c r="M147" s="22"/>
@@ -9195,7 +9205,7 @@
       <c r="G148" s="28"/>
       <c r="H148" s="28"/>
       <c r="I148" s="28"/>
-      <c r="J148" s="54"/>
+      <c r="J148" s="55"/>
       <c r="K148" s="23"/>
       <c r="L148" s="24"/>
       <c r="M148" s="22"/>
@@ -9212,7 +9222,7 @@
       <c r="G149" s="28"/>
       <c r="H149" s="28"/>
       <c r="I149" s="28"/>
-      <c r="J149" s="54"/>
+      <c r="J149" s="55"/>
       <c r="K149" s="23"/>
       <c r="L149" s="24"/>
       <c r="M149" s="22"/>
@@ -9229,7 +9239,7 @@
       <c r="G150" s="28"/>
       <c r="H150" s="28"/>
       <c r="I150" s="28"/>
-      <c r="J150" s="54"/>
+      <c r="J150" s="55"/>
       <c r="K150" s="23"/>
       <c r="L150" s="24"/>
       <c r="M150" s="22"/>
@@ -9246,7 +9256,7 @@
       <c r="G151" s="28"/>
       <c r="H151" s="28"/>
       <c r="I151" s="28"/>
-      <c r="J151" s="54"/>
+      <c r="J151" s="55"/>
       <c r="K151" s="23"/>
       <c r="L151" s="24"/>
       <c r="M151" s="22"/>
@@ -9263,7 +9273,7 @@
       <c r="G152" s="28"/>
       <c r="H152" s="28"/>
       <c r="I152" s="28"/>
-      <c r="J152" s="54"/>
+      <c r="J152" s="55"/>
       <c r="K152" s="23"/>
       <c r="L152" s="24"/>
       <c r="M152" s="22"/>
@@ -9280,7 +9290,7 @@
       <c r="G153" s="28"/>
       <c r="H153" s="28"/>
       <c r="I153" s="28"/>
-      <c r="J153" s="54"/>
+      <c r="J153" s="55"/>
       <c r="K153" s="23"/>
       <c r="L153" s="24"/>
       <c r="M153" s="22"/>
@@ -9297,7 +9307,7 @@
       <c r="G154" s="28"/>
       <c r="H154" s="28"/>
       <c r="I154" s="28"/>
-      <c r="J154" s="54"/>
+      <c r="J154" s="55"/>
       <c r="K154" s="23"/>
       <c r="L154" s="24"/>
       <c r="M154" s="22"/>
@@ -9314,7 +9324,7 @@
       <c r="G155" s="28"/>
       <c r="H155" s="28"/>
       <c r="I155" s="28"/>
-      <c r="J155" s="54"/>
+      <c r="J155" s="55"/>
       <c r="K155" s="23"/>
       <c r="L155" s="24"/>
       <c r="M155" s="22"/>
@@ -9331,7 +9341,7 @@
       <c r="G156" s="28"/>
       <c r="H156" s="28"/>
       <c r="I156" s="28"/>
-      <c r="J156" s="54"/>
+      <c r="J156" s="55"/>
       <c r="K156" s="23"/>
       <c r="L156" s="24"/>
       <c r="M156" s="22"/>
@@ -9348,7 +9358,7 @@
       <c r="G157" s="28"/>
       <c r="H157" s="28"/>
       <c r="I157" s="28"/>
-      <c r="J157" s="54"/>
+      <c r="J157" s="55"/>
       <c r="K157" s="23"/>
       <c r="L157" s="24"/>
       <c r="M157" s="22"/>
@@ -9365,7 +9375,7 @@
       <c r="G158" s="28"/>
       <c r="H158" s="28"/>
       <c r="I158" s="28"/>
-      <c r="J158" s="54"/>
+      <c r="J158" s="55"/>
       <c r="K158" s="23"/>
       <c r="L158" s="24"/>
       <c r="M158" s="22"/>
@@ -9382,7 +9392,7 @@
       <c r="G159" s="28"/>
       <c r="H159" s="28"/>
       <c r="I159" s="28"/>
-      <c r="J159" s="54"/>
+      <c r="J159" s="55"/>
       <c r="K159" s="23"/>
       <c r="L159" s="24"/>
       <c r="M159" s="22"/>
@@ -9399,7 +9409,7 @@
       <c r="G160" s="28"/>
       <c r="H160" s="28"/>
       <c r="I160" s="28"/>
-      <c r="J160" s="54"/>
+      <c r="J160" s="55"/>
       <c r="K160" s="23"/>
       <c r="L160" s="24"/>
       <c r="M160" s="22"/>
@@ -9416,7 +9426,7 @@
       <c r="G161" s="28"/>
       <c r="H161" s="28"/>
       <c r="I161" s="28"/>
-      <c r="J161" s="54"/>
+      <c r="J161" s="55"/>
       <c r="K161" s="23"/>
       <c r="L161" s="24"/>
       <c r="M161" s="22"/>
@@ -9433,7 +9443,7 @@
       <c r="G162" s="28"/>
       <c r="H162" s="28"/>
       <c r="I162" s="28"/>
-      <c r="J162" s="54"/>
+      <c r="J162" s="55"/>
       <c r="K162" s="23"/>
       <c r="L162" s="24"/>
       <c r="M162" s="22"/>
@@ -9450,7 +9460,7 @@
       <c r="G163" s="28"/>
       <c r="H163" s="28"/>
       <c r="I163" s="28"/>
-      <c r="J163" s="54"/>
+      <c r="J163" s="55"/>
       <c r="K163" s="23"/>
       <c r="L163" s="24"/>
       <c r="M163" s="22"/>
@@ -9467,7 +9477,7 @@
       <c r="G164" s="28"/>
       <c r="H164" s="28"/>
       <c r="I164" s="28"/>
-      <c r="J164" s="54"/>
+      <c r="J164" s="55"/>
       <c r="K164" s="23"/>
       <c r="L164" s="24"/>
       <c r="M164" s="22"/>
@@ -9484,7 +9494,7 @@
       <c r="G165" s="28"/>
       <c r="H165" s="28"/>
       <c r="I165" s="28"/>
-      <c r="J165" s="54"/>
+      <c r="J165" s="55"/>
       <c r="K165" s="23"/>
       <c r="L165" s="24"/>
       <c r="M165" s="22"/>
@@ -9501,7 +9511,7 @@
       <c r="G166" s="28"/>
       <c r="H166" s="28"/>
       <c r="I166" s="28"/>
-      <c r="J166" s="54"/>
+      <c r="J166" s="55"/>
       <c r="K166" s="23"/>
       <c r="L166" s="24"/>
       <c r="M166" s="22"/>
@@ -9518,7 +9528,7 @@
       <c r="G167" s="28"/>
       <c r="H167" s="28"/>
       <c r="I167" s="28"/>
-      <c r="J167" s="54"/>
+      <c r="J167" s="55"/>
       <c r="K167" s="23"/>
       <c r="L167" s="24"/>
       <c r="M167" s="22"/>
@@ -9535,7 +9545,7 @@
       <c r="G168" s="28"/>
       <c r="H168" s="28"/>
       <c r="I168" s="28"/>
-      <c r="J168" s="54"/>
+      <c r="J168" s="55"/>
       <c r="K168" s="23"/>
       <c r="L168" s="24"/>
       <c r="M168" s="22"/>
@@ -9552,7 +9562,7 @@
       <c r="G169" s="28"/>
       <c r="H169" s="28"/>
       <c r="I169" s="28"/>
-      <c r="J169" s="54"/>
+      <c r="J169" s="55"/>
       <c r="K169" s="23"/>
       <c r="L169" s="24"/>
       <c r="M169" s="22"/>
@@ -9569,7 +9579,7 @@
       <c r="G170" s="28"/>
       <c r="H170" s="28"/>
       <c r="I170" s="28"/>
-      <c r="J170" s="54"/>
+      <c r="J170" s="55"/>
       <c r="K170" s="23"/>
       <c r="L170" s="24"/>
       <c r="M170" s="22"/>
@@ -9586,7 +9596,7 @@
       <c r="G171" s="28"/>
       <c r="H171" s="28"/>
       <c r="I171" s="28"/>
-      <c r="J171" s="54"/>
+      <c r="J171" s="55"/>
       <c r="K171" s="23"/>
       <c r="L171" s="24"/>
       <c r="M171" s="22"/>
@@ -9603,7 +9613,7 @@
       <c r="G172" s="28"/>
       <c r="H172" s="28"/>
       <c r="I172" s="28"/>
-      <c r="J172" s="54"/>
+      <c r="J172" s="55"/>
       <c r="K172" s="23"/>
       <c r="L172" s="24"/>
       <c r="M172" s="22"/>
@@ -9620,7 +9630,7 @@
       <c r="G173" s="28"/>
       <c r="H173" s="28"/>
       <c r="I173" s="28"/>
-      <c r="J173" s="54"/>
+      <c r="J173" s="55"/>
       <c r="K173" s="23"/>
       <c r="L173" s="24"/>
       <c r="M173" s="22"/>
@@ -9637,7 +9647,7 @@
       <c r="G174" s="28"/>
       <c r="H174" s="28"/>
       <c r="I174" s="28"/>
-      <c r="J174" s="54"/>
+      <c r="J174" s="55"/>
       <c r="K174" s="23"/>
       <c r="L174" s="24"/>
       <c r="M174" s="22"/>
@@ -9654,7 +9664,7 @@
       <c r="G175" s="28"/>
       <c r="H175" s="28"/>
       <c r="I175" s="28"/>
-      <c r="J175" s="54"/>
+      <c r="J175" s="55"/>
       <c r="K175" s="23"/>
       <c r="L175" s="24"/>
       <c r="M175" s="22"/>
@@ -9671,7 +9681,7 @@
       <c r="G176" s="28"/>
       <c r="H176" s="28"/>
       <c r="I176" s="28"/>
-      <c r="J176" s="54"/>
+      <c r="J176" s="55"/>
       <c r="K176" s="23"/>
       <c r="L176" s="24"/>
       <c r="M176" s="22"/>
@@ -9688,7 +9698,7 @@
       <c r="G177" s="28"/>
       <c r="H177" s="28"/>
       <c r="I177" s="28"/>
-      <c r="J177" s="54"/>
+      <c r="J177" s="55"/>
       <c r="K177" s="23"/>
       <c r="L177" s="24"/>
       <c r="M177" s="22"/>
@@ -9705,7 +9715,7 @@
       <c r="G178" s="28"/>
       <c r="H178" s="28"/>
       <c r="I178" s="28"/>
-      <c r="J178" s="54"/>
+      <c r="J178" s="55"/>
       <c r="K178" s="23"/>
       <c r="L178" s="24"/>
       <c r="M178" s="22"/>
@@ -9722,7 +9732,7 @@
       <c r="G179" s="28"/>
       <c r="H179" s="28"/>
       <c r="I179" s="28"/>
-      <c r="J179" s="54"/>
+      <c r="J179" s="55"/>
       <c r="K179" s="23"/>
       <c r="L179" s="24"/>
       <c r="M179" s="22"/>
@@ -9739,7 +9749,7 @@
       <c r="G180" s="28"/>
       <c r="H180" s="28"/>
       <c r="I180" s="28"/>
-      <c r="J180" s="54"/>
+      <c r="J180" s="55"/>
       <c r="K180" s="23"/>
       <c r="L180" s="24"/>
       <c r="M180" s="22"/>
@@ -9756,7 +9766,7 @@
       <c r="G181" s="28"/>
       <c r="H181" s="28"/>
       <c r="I181" s="28"/>
-      <c r="J181" s="54"/>
+      <c r="J181" s="55"/>
       <c r="K181" s="23"/>
       <c r="L181" s="24"/>
       <c r="M181" s="22"/>
@@ -9773,7 +9783,7 @@
       <c r="G182" s="28"/>
       <c r="H182" s="28"/>
       <c r="I182" s="28"/>
-      <c r="J182" s="54"/>
+      <c r="J182" s="55"/>
       <c r="K182" s="23"/>
       <c r="L182" s="24"/>
       <c r="M182" s="22"/>
@@ -9790,7 +9800,7 @@
       <c r="G183" s="28"/>
       <c r="H183" s="28"/>
       <c r="I183" s="28"/>
-      <c r="J183" s="54"/>
+      <c r="J183" s="55"/>
       <c r="K183" s="23"/>
       <c r="L183" s="24"/>
       <c r="M183" s="22"/>
@@ -9807,7 +9817,7 @@
       <c r="G184" s="28"/>
       <c r="H184" s="28"/>
       <c r="I184" s="28"/>
-      <c r="J184" s="54"/>
+      <c r="J184" s="55"/>
       <c r="K184" s="23"/>
       <c r="L184" s="24"/>
       <c r="M184" s="22"/>
@@ -9824,7 +9834,7 @@
       <c r="G185" s="28"/>
       <c r="H185" s="28"/>
       <c r="I185" s="28"/>
-      <c r="J185" s="54"/>
+      <c r="J185" s="55"/>
       <c r="K185" s="23"/>
       <c r="L185" s="24"/>
       <c r="M185" s="22"/>
@@ -9841,7 +9851,7 @@
       <c r="G186" s="28"/>
       <c r="H186" s="28"/>
       <c r="I186" s="28"/>
-      <c r="J186" s="54"/>
+      <c r="J186" s="55"/>
       <c r="K186" s="23"/>
       <c r="L186" s="24"/>
       <c r="M186" s="22"/>
@@ -9858,7 +9868,7 @@
       <c r="G187" s="28"/>
       <c r="H187" s="28"/>
       <c r="I187" s="28"/>
-      <c r="J187" s="54"/>
+      <c r="J187" s="55"/>
       <c r="K187" s="23"/>
       <c r="L187" s="24"/>
       <c r="M187" s="22"/>
@@ -9875,7 +9885,7 @@
       <c r="G188" s="28"/>
       <c r="H188" s="28"/>
       <c r="I188" s="28"/>
-      <c r="J188" s="54"/>
+      <c r="J188" s="55"/>
       <c r="K188" s="23"/>
       <c r="L188" s="24"/>
       <c r="M188" s="22"/>
@@ -9938,10 +9948,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O183"/>
+  <dimension ref="A1:O185"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>
@@ -9985,14 +9995,14 @@
       <c r="I1" s="15" t="s">
         <v>731</v>
       </c>
-      <c r="J1" s="43"/>
+      <c r="J1" s="44"/>
       <c r="K1" s="23"/>
       <c r="L1" s="15" t="s">
         <v>732</v>
       </c>
       <c r="M1" s="15"/>
       <c r="N1" s="15"/>
-      <c r="O1" s="44"/>
+      <c r="O1" s="45"/>
     </row>
     <row r="2" s="1" customFormat="1" ht="15.25" spans="1:15">
       <c r="A2" s="16" t="s">
@@ -10006,12 +10016,12 @@
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
       <c r="I2" s="19"/>
-      <c r="J2" s="43"/>
+      <c r="J2" s="44"/>
       <c r="K2" s="23"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
     </row>
     <row r="3" s="1" customFormat="1" ht="10" customHeight="1" spans="1:15">
       <c r="A3" s="20"/>
@@ -10023,7 +10033,7 @@
       <c r="G3" s="24"/>
       <c r="H3" s="24"/>
       <c r="I3" s="24"/>
-      <c r="J3" s="47"/>
+      <c r="J3" s="48"/>
       <c r="K3" s="23"/>
       <c r="L3" s="24"/>
       <c r="M3" s="22"/>
@@ -10058,10 +10068,10 @@
       <c r="I4" s="25" t="s">
         <v>741</v>
       </c>
-      <c r="J4" s="48" t="s">
+      <c r="J4" s="49" t="s">
         <v>742</v>
       </c>
-      <c r="K4" s="49"/>
+      <c r="K4" s="50"/>
       <c r="L4" s="25" t="s">
         <v>743</v>
       </c>
@@ -10097,12 +10107,12 @@
       <c r="G5" s="30"/>
       <c r="H5" s="30"/>
       <c r="I5" s="30"/>
-      <c r="J5" s="50"/>
-      <c r="K5" s="51"/>
-      <c r="L5" s="52"/>
-      <c r="M5" s="53"/>
-      <c r="N5" s="52"/>
-      <c r="O5" s="51"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="52"/>
+      <c r="L5" s="53"/>
+      <c r="M5" s="54"/>
+      <c r="N5" s="53"/>
+      <c r="O5" s="52"/>
     </row>
     <row r="6" s="3" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A6" s="20"/>
@@ -10124,12 +10134,12 @@
       <c r="G6" s="30"/>
       <c r="H6" s="30"/>
       <c r="I6" s="30"/>
-      <c r="J6" s="50"/>
-      <c r="K6" s="51"/>
-      <c r="L6" s="52"/>
-      <c r="M6" s="53"/>
-      <c r="N6" s="52"/>
-      <c r="O6" s="51"/>
+      <c r="J6" s="51"/>
+      <c r="K6" s="52"/>
+      <c r="L6" s="53"/>
+      <c r="M6" s="54"/>
+      <c r="N6" s="53"/>
+      <c r="O6" s="52"/>
     </row>
     <row r="7" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A7" s="20"/>
@@ -10151,7 +10161,7 @@
       <c r="G7" s="28"/>
       <c r="H7" s="28"/>
       <c r="I7" s="28"/>
-      <c r="J7" s="54"/>
+      <c r="J7" s="55"/>
       <c r="K7" s="23"/>
       <c r="L7" s="24"/>
       <c r="M7" s="22"/>
@@ -10176,7 +10186,7 @@
       <c r="G8" s="28"/>
       <c r="H8" s="28"/>
       <c r="I8" s="28"/>
-      <c r="J8" s="54"/>
+      <c r="J8" s="55"/>
       <c r="K8" s="23"/>
       <c r="L8" s="24"/>
       <c r="M8" s="22"/>
@@ -10201,7 +10211,7 @@
       <c r="G9" s="28"/>
       <c r="H9" s="28"/>
       <c r="I9" s="28"/>
-      <c r="J9" s="54"/>
+      <c r="J9" s="55"/>
       <c r="K9" s="23"/>
       <c r="L9" s="24"/>
       <c r="M9" s="22"/>
@@ -10228,7 +10238,7 @@
       <c r="G10" s="28"/>
       <c r="H10" s="28"/>
       <c r="I10" s="28"/>
-      <c r="J10" s="54"/>
+      <c r="J10" s="55"/>
       <c r="K10" s="23"/>
       <c r="L10" s="24"/>
       <c r="M10" s="22"/>
@@ -10253,7 +10263,7 @@
       <c r="G11" s="28"/>
       <c r="H11" s="28"/>
       <c r="I11" s="28"/>
-      <c r="J11" s="54"/>
+      <c r="J11" s="55"/>
       <c r="K11" s="23"/>
       <c r="L11" s="24"/>
       <c r="M11" s="22"/>
@@ -10282,7 +10292,7 @@
       <c r="G12" s="28"/>
       <c r="H12" s="28"/>
       <c r="I12" s="28"/>
-      <c r="J12" s="54"/>
+      <c r="J12" s="55"/>
       <c r="K12" s="23"/>
       <c r="L12" s="24"/>
       <c r="M12" s="22"/>
@@ -10307,7 +10317,7 @@
       <c r="G13" s="28"/>
       <c r="H13" s="28"/>
       <c r="I13" s="28"/>
-      <c r="J13" s="54"/>
+      <c r="J13" s="55"/>
       <c r="K13" s="23"/>
       <c r="L13" s="24"/>
       <c r="M13" s="22"/>
@@ -10334,7 +10344,7 @@
       <c r="G14" s="28"/>
       <c r="H14" s="28"/>
       <c r="I14" s="28"/>
-      <c r="J14" s="54"/>
+      <c r="J14" s="55"/>
       <c r="K14" s="23"/>
       <c r="L14" s="24"/>
       <c r="M14" s="22"/>
@@ -10359,7 +10369,7 @@
       <c r="G15" s="28"/>
       <c r="H15" s="28"/>
       <c r="I15" s="28"/>
-      <c r="J15" s="54"/>
+      <c r="J15" s="55"/>
       <c r="K15" s="23"/>
       <c r="L15" s="24"/>
       <c r="M15" s="22"/>
@@ -10384,7 +10394,7 @@
       <c r="G16" s="28"/>
       <c r="H16" s="28"/>
       <c r="I16" s="28"/>
-      <c r="J16" s="54"/>
+      <c r="J16" s="55"/>
       <c r="K16" s="23"/>
       <c r="L16" s="24"/>
       <c r="M16" s="22"/>
@@ -10411,7 +10421,7 @@
       <c r="G17" s="28"/>
       <c r="H17" s="28"/>
       <c r="I17" s="28"/>
-      <c r="J17" s="54"/>
+      <c r="J17" s="55"/>
       <c r="K17" s="23"/>
       <c r="L17" s="24"/>
       <c r="M17" s="22"/>
@@ -10438,7 +10448,7 @@
       <c r="G18" s="28"/>
       <c r="H18" s="28"/>
       <c r="I18" s="28"/>
-      <c r="J18" s="54"/>
+      <c r="J18" s="55"/>
       <c r="K18" s="23"/>
       <c r="L18" s="24"/>
       <c r="M18" s="22"/>
@@ -10465,7 +10475,7 @@
       <c r="G19" s="28"/>
       <c r="H19" s="28"/>
       <c r="I19" s="28"/>
-      <c r="J19" s="54"/>
+      <c r="J19" s="55"/>
       <c r="K19" s="23"/>
       <c r="L19" s="24"/>
       <c r="M19" s="22"/>
@@ -10491,7 +10501,7 @@
       <c r="G20" s="28"/>
       <c r="H20" s="28"/>
       <c r="I20" s="28"/>
-      <c r="J20" s="54"/>
+      <c r="J20" s="55"/>
       <c r="K20" s="23"/>
       <c r="L20" s="24"/>
       <c r="M20" s="22"/>
@@ -10516,7 +10526,7 @@
       <c r="G21" s="28"/>
       <c r="H21" s="28"/>
       <c r="I21" s="28"/>
-      <c r="J21" s="54"/>
+      <c r="J21" s="55"/>
       <c r="K21" s="23"/>
       <c r="L21" s="24"/>
       <c r="M21" s="22"/>
@@ -10540,7 +10550,7 @@
       <c r="G22" s="28"/>
       <c r="H22" s="28"/>
       <c r="I22" s="28"/>
-      <c r="J22" s="54"/>
+      <c r="J22" s="55"/>
       <c r="K22" s="23"/>
       <c r="L22" s="24"/>
       <c r="M22" s="22"/>
@@ -10567,7 +10577,7 @@
       <c r="G23" s="28"/>
       <c r="H23" s="28"/>
       <c r="I23" s="28"/>
-      <c r="J23" s="54"/>
+      <c r="J23" s="55"/>
       <c r="K23" s="23"/>
       <c r="L23" s="24"/>
       <c r="M23" s="22"/>
@@ -10593,7 +10603,7 @@
       <c r="G24" s="28"/>
       <c r="H24" s="28"/>
       <c r="I24" s="28"/>
-      <c r="J24" s="54"/>
+      <c r="J24" s="55"/>
       <c r="K24" s="23"/>
       <c r="L24" s="24"/>
       <c r="M24" s="22"/>
@@ -10620,7 +10630,7 @@
       <c r="G25" s="28"/>
       <c r="H25" s="28"/>
       <c r="I25" s="28"/>
-      <c r="J25" s="54"/>
+      <c r="J25" s="55"/>
       <c r="K25" s="23"/>
       <c r="L25" s="24"/>
       <c r="M25" s="22"/>
@@ -10647,7 +10657,7 @@
       <c r="G26" s="28"/>
       <c r="H26" s="28"/>
       <c r="I26" s="28"/>
-      <c r="J26" s="54"/>
+      <c r="J26" s="55"/>
       <c r="K26" s="23"/>
       <c r="L26" s="24"/>
       <c r="M26" s="22"/>
@@ -10673,7 +10683,7 @@
       <c r="G27" s="28"/>
       <c r="H27" s="28"/>
       <c r="I27" s="28"/>
-      <c r="J27" s="54"/>
+      <c r="J27" s="55"/>
       <c r="K27" s="23"/>
       <c r="L27" s="24"/>
       <c r="M27" s="22"/>
@@ -10698,7 +10708,7 @@
       <c r="G28" s="28"/>
       <c r="H28" s="28"/>
       <c r="I28" s="28"/>
-      <c r="J28" s="54"/>
+      <c r="J28" s="55"/>
       <c r="K28" s="23"/>
       <c r="L28" s="24"/>
       <c r="M28" s="22"/>
@@ -10725,12 +10735,12 @@
       <c r="G29" s="41"/>
       <c r="H29" s="41"/>
       <c r="I29" s="41"/>
-      <c r="J29" s="55"/>
-      <c r="K29" s="56"/>
-      <c r="L29" s="57"/>
-      <c r="M29" s="58"/>
-      <c r="N29" s="57"/>
-      <c r="O29" s="56"/>
+      <c r="J29" s="56"/>
+      <c r="K29" s="57"/>
+      <c r="L29" s="58"/>
+      <c r="M29" s="59"/>
+      <c r="N29" s="58"/>
+      <c r="O29" s="57"/>
     </row>
     <row r="30" s="4" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A30" s="38"/>
@@ -10741,68 +10751,66 @@
         <v>30</v>
       </c>
       <c r="D30" s="41" t="s">
-        <v>253</v>
-      </c>
-      <c r="E30" s="41" t="s">
-        <v>800</v>
+        <v>553</v>
+      </c>
+      <c r="E30" s="43" t="s">
+        <v>798</v>
       </c>
       <c r="F30" s="42"/>
       <c r="G30" s="41"/>
       <c r="H30" s="41"/>
       <c r="I30" s="41"/>
-      <c r="J30" s="55"/>
-      <c r="K30" s="56"/>
-      <c r="L30" s="57"/>
-      <c r="M30" s="58"/>
-      <c r="N30" s="57"/>
-      <c r="O30" s="56"/>
-    </row>
-    <row r="31" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A31" s="20"/>
-      <c r="B31" s="31" t="s">
+      <c r="J30" s="56"/>
+      <c r="K30" s="57"/>
+      <c r="L30" s="58"/>
+      <c r="M30" s="59"/>
+      <c r="N30" s="58"/>
+      <c r="O30" s="57"/>
+    </row>
+    <row r="31" s="4" customFormat="1" ht="23" customHeight="1" spans="1:15">
+      <c r="A31" s="38"/>
+      <c r="B31" s="39" t="s">
         <v>808</v>
       </c>
-      <c r="C31" s="27" t="s">
+      <c r="C31" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="D31" s="28" t="s">
-        <v>363</v>
-      </c>
-      <c r="E31" s="28" t="s">
-        <v>789</v>
-      </c>
-      <c r="F31" s="29"/>
-      <c r="G31" s="28"/>
-      <c r="H31" s="28"/>
-      <c r="I31" s="28"/>
-      <c r="J31" s="54"/>
-      <c r="K31" s="23"/>
-      <c r="L31" s="24"/>
-      <c r="M31" s="22"/>
-      <c r="N31" s="24"/>
-      <c r="O31" s="23"/>
+      <c r="D31" s="41" t="s">
+        <v>253</v>
+      </c>
+      <c r="E31" s="41" t="s">
+        <v>800</v>
+      </c>
+      <c r="F31" s="42"/>
+      <c r="G31" s="41"/>
+      <c r="H31" s="41"/>
+      <c r="I31" s="41"/>
+      <c r="J31" s="56"/>
+      <c r="K31" s="57"/>
+      <c r="L31" s="58"/>
+      <c r="M31" s="59"/>
+      <c r="N31" s="58"/>
+      <c r="O31" s="57"/>
     </row>
     <row r="32" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A32" s="20" t="s">
+      <c r="A32" s="20"/>
+      <c r="B32" s="39" t="s">
         <v>809</v>
       </c>
-      <c r="B32" s="31" t="s">
-        <v>808</v>
-      </c>
-      <c r="C32" s="27" t="s">
+      <c r="C32" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="D32" s="28" t="s">
-        <v>363</v>
-      </c>
-      <c r="E32" s="28" t="s">
-        <v>789</v>
+      <c r="D32" s="41" t="s">
+        <v>553</v>
+      </c>
+      <c r="E32" s="43" t="s">
+        <v>801</v>
       </c>
       <c r="F32" s="29"/>
       <c r="G32" s="28"/>
       <c r="H32" s="28"/>
       <c r="I32" s="28"/>
-      <c r="J32" s="54"/>
+      <c r="J32" s="55"/>
       <c r="K32" s="23"/>
       <c r="L32" s="24"/>
       <c r="M32" s="22"/>
@@ -10812,24 +10820,22 @@
     <row r="33" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A33" s="20"/>
       <c r="B33" s="31" t="s">
-        <v>796</v>
+        <v>810</v>
       </c>
       <c r="C33" s="27" t="s">
         <v>30</v>
       </c>
       <c r="D33" s="28" t="s">
-        <v>707</v>
+        <v>363</v>
       </c>
       <c r="E33" s="28" t="s">
-        <v>797</v>
-      </c>
-      <c r="F33" s="37" t="s">
-        <v>810</v>
-      </c>
+        <v>789</v>
+      </c>
+      <c r="F33" s="29"/>
       <c r="G33" s="28"/>
       <c r="H33" s="28"/>
       <c r="I33" s="28"/>
-      <c r="J33" s="54"/>
+      <c r="J33" s="55"/>
       <c r="K33" s="23"/>
       <c r="L33" s="24"/>
       <c r="M33" s="22"/>
@@ -10837,24 +10843,26 @@
       <c r="O33" s="23"/>
     </row>
     <row r="34" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A34" s="20"/>
+      <c r="A34" s="20" t="s">
+        <v>811</v>
+      </c>
       <c r="B34" s="31" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="C34" s="27" t="s">
         <v>30</v>
       </c>
       <c r="D34" s="28" t="s">
-        <v>253</v>
+        <v>363</v>
       </c>
       <c r="E34" s="28" t="s">
-        <v>812</v>
-      </c>
-      <c r="F34" s="37"/>
+        <v>789</v>
+      </c>
+      <c r="F34" s="29"/>
       <c r="G34" s="28"/>
       <c r="H34" s="28"/>
       <c r="I34" s="28"/>
-      <c r="J34" s="54"/>
+      <c r="J34" s="55"/>
       <c r="K34" s="23"/>
       <c r="L34" s="24"/>
       <c r="M34" s="22"/>
@@ -10864,7 +10872,7 @@
     <row r="35" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A35" s="20"/>
       <c r="B35" s="31" t="s">
-        <v>799</v>
+        <v>796</v>
       </c>
       <c r="C35" s="27" t="s">
         <v>30</v>
@@ -10873,15 +10881,15 @@
         <v>707</v>
       </c>
       <c r="E35" s="28" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
       <c r="F35" s="37" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="G35" s="28"/>
       <c r="H35" s="28"/>
       <c r="I35" s="28"/>
-      <c r="J35" s="54"/>
+      <c r="J35" s="55"/>
       <c r="K35" s="23"/>
       <c r="L35" s="24"/>
       <c r="M35" s="22"/>
@@ -10891,7 +10899,7 @@
     <row r="36" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A36" s="20"/>
       <c r="B36" s="31" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="C36" s="27" t="s">
         <v>30</v>
@@ -10900,13 +10908,13 @@
         <v>253</v>
       </c>
       <c r="E36" s="28" t="s">
-        <v>815</v>
-      </c>
-      <c r="F36" s="29"/>
+        <v>814</v>
+      </c>
+      <c r="F36" s="37"/>
       <c r="G36" s="28"/>
       <c r="H36" s="28"/>
       <c r="I36" s="28"/>
-      <c r="J36" s="54"/>
+      <c r="J36" s="55"/>
       <c r="K36" s="23"/>
       <c r="L36" s="24"/>
       <c r="M36" s="22"/>
@@ -10916,24 +10924,24 @@
     <row r="37" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A37" s="20"/>
       <c r="B37" s="31" t="s">
-        <v>816</v>
+        <v>799</v>
       </c>
       <c r="C37" s="27" t="s">
         <v>30</v>
       </c>
       <c r="D37" s="28" t="s">
-        <v>576</v>
+        <v>707</v>
       </c>
       <c r="E37" s="28" t="s">
-        <v>817</v>
-      </c>
-      <c r="F37" s="29">
-        <v>3000</v>
+        <v>800</v>
+      </c>
+      <c r="F37" s="37" t="s">
+        <v>815</v>
       </c>
       <c r="G37" s="28"/>
       <c r="H37" s="28"/>
       <c r="I37" s="28"/>
-      <c r="J37" s="54"/>
+      <c r="J37" s="55"/>
       <c r="K37" s="23"/>
       <c r="L37" s="24"/>
       <c r="M37" s="22"/>
@@ -10943,7 +10951,7 @@
     <row r="38" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A38" s="20"/>
       <c r="B38" s="31" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="C38" s="27" t="s">
         <v>30</v>
@@ -10952,13 +10960,13 @@
         <v>253</v>
       </c>
       <c r="E38" s="28" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="F38" s="29"/>
       <c r="G38" s="28"/>
       <c r="H38" s="28"/>
       <c r="I38" s="28"/>
-      <c r="J38" s="54"/>
+      <c r="J38" s="55"/>
       <c r="K38" s="23"/>
       <c r="L38" s="24"/>
       <c r="M38" s="22"/>
@@ -10966,26 +10974,26 @@
       <c r="O38" s="23"/>
     </row>
     <row r="39" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A39" s="20" t="s">
-        <v>820</v>
-      </c>
+      <c r="A39" s="20"/>
       <c r="B39" s="31" t="s">
-        <v>808</v>
+        <v>818</v>
       </c>
       <c r="C39" s="27" t="s">
         <v>30</v>
       </c>
       <c r="D39" s="28" t="s">
-        <v>363</v>
+        <v>576</v>
       </c>
       <c r="E39" s="28" t="s">
-        <v>789</v>
-      </c>
-      <c r="F39" s="29"/>
+        <v>819</v>
+      </c>
+      <c r="F39" s="29">
+        <v>3000</v>
+      </c>
       <c r="G39" s="28"/>
       <c r="H39" s="28"/>
       <c r="I39" s="28"/>
-      <c r="J39" s="54"/>
+      <c r="J39" s="55"/>
       <c r="K39" s="23"/>
       <c r="L39" s="24"/>
       <c r="M39" s="22"/>
@@ -10995,24 +11003,22 @@
     <row r="40" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A40" s="20"/>
       <c r="B40" s="31" t="s">
-        <v>796</v>
+        <v>820</v>
       </c>
       <c r="C40" s="27" t="s">
         <v>30</v>
       </c>
       <c r="D40" s="28" t="s">
-        <v>707</v>
+        <v>253</v>
       </c>
       <c r="E40" s="28" t="s">
-        <v>797</v>
-      </c>
-      <c r="F40" s="37" t="s">
-        <v>798</v>
-      </c>
+        <v>821</v>
+      </c>
+      <c r="F40" s="29"/>
       <c r="G40" s="28"/>
       <c r="H40" s="28"/>
       <c r="I40" s="28"/>
-      <c r="J40" s="54"/>
+      <c r="J40" s="55"/>
       <c r="K40" s="23"/>
       <c r="L40" s="24"/>
       <c r="M40" s="22"/>
@@ -11020,26 +11026,26 @@
       <c r="O40" s="23"/>
     </row>
     <row r="41" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A41" s="20"/>
+      <c r="A41" s="20" t="s">
+        <v>822</v>
+      </c>
       <c r="B41" s="31" t="s">
-        <v>799</v>
+        <v>810</v>
       </c>
       <c r="C41" s="27" t="s">
         <v>30</v>
       </c>
       <c r="D41" s="28" t="s">
-        <v>707</v>
+        <v>363</v>
       </c>
       <c r="E41" s="28" t="s">
-        <v>800</v>
-      </c>
-      <c r="F41" s="37" t="s">
-        <v>801</v>
-      </c>
+        <v>789</v>
+      </c>
+      <c r="F41" s="29"/>
       <c r="G41" s="28"/>
       <c r="H41" s="28"/>
       <c r="I41" s="28"/>
-      <c r="J41" s="54"/>
+      <c r="J41" s="55"/>
       <c r="K41" s="23"/>
       <c r="L41" s="24"/>
       <c r="M41" s="22"/>
@@ -11049,24 +11055,24 @@
     <row r="42" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A42" s="20"/>
       <c r="B42" s="31" t="s">
-        <v>821</v>
+        <v>796</v>
       </c>
       <c r="C42" s="27" t="s">
         <v>30</v>
       </c>
       <c r="D42" s="28" t="s">
-        <v>576</v>
+        <v>707</v>
       </c>
       <c r="E42" s="28" t="s">
-        <v>817</v>
-      </c>
-      <c r="F42" s="29">
-        <v>3000</v>
+        <v>797</v>
+      </c>
+      <c r="F42" s="37" t="s">
+        <v>798</v>
       </c>
       <c r="G42" s="28"/>
       <c r="H42" s="28"/>
       <c r="I42" s="28"/>
-      <c r="J42" s="54"/>
+      <c r="J42" s="55"/>
       <c r="K42" s="23"/>
       <c r="L42" s="24"/>
       <c r="M42" s="22"/>
@@ -11076,29 +11082,31 @@
     <row r="43" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A43" s="20"/>
       <c r="B43" s="31" t="s">
-        <v>822</v>
+        <v>799</v>
       </c>
       <c r="C43" s="27" t="s">
         <v>30</v>
       </c>
       <c r="D43" s="28" t="s">
-        <v>253</v>
+        <v>707</v>
       </c>
       <c r="E43" s="28" t="s">
-        <v>767</v>
-      </c>
-      <c r="F43" s="29"/>
+        <v>800</v>
+      </c>
+      <c r="F43" s="37" t="s">
+        <v>801</v>
+      </c>
       <c r="G43" s="28"/>
       <c r="H43" s="28"/>
       <c r="I43" s="28"/>
-      <c r="J43" s="54"/>
+      <c r="J43" s="55"/>
       <c r="K43" s="23"/>
       <c r="L43" s="24"/>
       <c r="M43" s="22"/>
       <c r="N43" s="24"/>
       <c r="O43" s="23"/>
     </row>
-    <row r="44" s="1" customFormat="1" ht="24" customHeight="1" spans="1:15">
+    <row r="44" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A44" s="20"/>
       <c r="B44" s="31" t="s">
         <v>823</v>
@@ -11107,174 +11115,172 @@
         <v>30</v>
       </c>
       <c r="D44" s="28" t="s">
-        <v>363</v>
+        <v>576</v>
       </c>
       <c r="E44" s="28" t="s">
-        <v>824</v>
-      </c>
-      <c r="F44" s="29"/>
+        <v>819</v>
+      </c>
+      <c r="F44" s="29">
+        <v>3000</v>
+      </c>
       <c r="G44" s="28"/>
       <c r="H44" s="28"/>
       <c r="I44" s="28"/>
-      <c r="J44" s="54"/>
+      <c r="J44" s="55"/>
       <c r="K44" s="23"/>
       <c r="L44" s="24"/>
       <c r="M44" s="22"/>
       <c r="N44" s="24"/>
       <c r="O44" s="23"/>
     </row>
-    <row r="45" s="1" customFormat="1" ht="24" customHeight="1" spans="1:15">
+    <row r="45" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A45" s="20"/>
       <c r="B45" s="31" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C45" s="27" t="s">
         <v>30</v>
       </c>
       <c r="D45" s="28" t="s">
-        <v>483</v>
+        <v>253</v>
       </c>
       <c r="E45" s="28" t="s">
-        <v>772</v>
-      </c>
-      <c r="F45" s="29" t="s">
-        <v>773</v>
-      </c>
+        <v>767</v>
+      </c>
+      <c r="F45" s="29"/>
       <c r="G45" s="28"/>
       <c r="H45" s="28"/>
       <c r="I45" s="28"/>
-      <c r="J45" s="54"/>
+      <c r="J45" s="55"/>
       <c r="K45" s="23"/>
       <c r="L45" s="24"/>
       <c r="M45" s="22"/>
       <c r="N45" s="24"/>
       <c r="O45" s="23"/>
     </row>
-    <row r="46" s="1" customFormat="1" ht="19" customHeight="1" spans="1:15">
+    <row r="46" s="1" customFormat="1" ht="24" customHeight="1" spans="1:15">
       <c r="A46" s="20"/>
       <c r="B46" s="31" t="s">
+        <v>825</v>
+      </c>
+      <c r="C46" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D46" s="28" t="s">
+        <v>363</v>
+      </c>
+      <c r="E46" s="28" t="s">
         <v>826</v>
       </c>
-      <c r="C46" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="D46" s="33" t="s">
-        <v>471</v>
-      </c>
-      <c r="E46" s="33" t="s">
-        <v>775</v>
-      </c>
-      <c r="F46" s="34" t="s">
-        <v>776</v>
-      </c>
+      <c r="F46" s="29"/>
       <c r="G46" s="28"/>
       <c r="H46" s="28"/>
       <c r="I46" s="28"/>
-      <c r="J46" s="54"/>
+      <c r="J46" s="55"/>
       <c r="K46" s="23"/>
       <c r="L46" s="24"/>
       <c r="M46" s="22"/>
       <c r="N46" s="24"/>
       <c r="O46" s="23"/>
     </row>
-    <row r="47" s="1" customFormat="1" ht="20" customHeight="1" spans="1:15">
+    <row r="47" s="1" customFormat="1" ht="24" customHeight="1" spans="1:15">
       <c r="A47" s="20"/>
-      <c r="B47" s="31"/>
-      <c r="C47" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="D47" s="33" t="s">
-        <v>465</v>
-      </c>
-      <c r="E47" s="33" t="s">
-        <v>777</v>
-      </c>
-      <c r="F47" s="34" t="s">
-        <v>778</v>
+      <c r="B47" s="31" t="s">
+        <v>827</v>
+      </c>
+      <c r="C47" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D47" s="28" t="s">
+        <v>483</v>
+      </c>
+      <c r="E47" s="28" t="s">
+        <v>772</v>
+      </c>
+      <c r="F47" s="29" t="s">
+        <v>773</v>
       </c>
       <c r="G47" s="28"/>
       <c r="H47" s="28"/>
       <c r="I47" s="28"/>
-      <c r="J47" s="54"/>
+      <c r="J47" s="55"/>
       <c r="K47" s="23"/>
       <c r="L47" s="24"/>
       <c r="M47" s="22"/>
       <c r="N47" s="24"/>
       <c r="O47" s="23"/>
     </row>
-    <row r="48" s="1" customFormat="1" ht="17" customHeight="1" spans="1:15">
+    <row r="48" s="1" customFormat="1" ht="19" customHeight="1" spans="1:15">
       <c r="A48" s="20"/>
-      <c r="B48" s="31"/>
+      <c r="B48" s="31" t="s">
+        <v>828</v>
+      </c>
       <c r="C48" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="D48" s="35" t="s">
-        <v>49</v>
+      <c r="D48" s="33" t="s">
+        <v>471</v>
       </c>
       <c r="E48" s="33" t="s">
-        <v>779</v>
-      </c>
-      <c r="F48" s="28" t="s">
-        <v>780</v>
+        <v>775</v>
+      </c>
+      <c r="F48" s="34" t="s">
+        <v>776</v>
       </c>
       <c r="G48" s="28"/>
       <c r="H48" s="28"/>
       <c r="I48" s="28"/>
-      <c r="J48" s="54"/>
+      <c r="J48" s="55"/>
       <c r="K48" s="23"/>
       <c r="L48" s="24"/>
       <c r="M48" s="22"/>
       <c r="N48" s="24"/>
       <c r="O48" s="23"/>
     </row>
-    <row r="49" s="1" customFormat="1" ht="22" customHeight="1" spans="1:15">
+    <row r="49" s="1" customFormat="1" ht="20" customHeight="1" spans="1:15">
       <c r="A49" s="20"/>
-      <c r="B49" s="31" t="s">
-        <v>781</v>
-      </c>
+      <c r="B49" s="31"/>
       <c r="C49" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="D49" s="35" t="s">
-        <v>302</v>
+        <v>5</v>
+      </c>
+      <c r="D49" s="33" t="s">
+        <v>465</v>
       </c>
       <c r="E49" s="33" t="s">
-        <v>775</v>
+        <v>777</v>
       </c>
       <c r="F49" s="34" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
       <c r="G49" s="28"/>
       <c r="H49" s="28"/>
       <c r="I49" s="28"/>
-      <c r="J49" s="54"/>
+      <c r="J49" s="55"/>
       <c r="K49" s="23"/>
       <c r="L49" s="24"/>
       <c r="M49" s="22"/>
       <c r="N49" s="24"/>
       <c r="O49" s="23"/>
     </row>
-    <row r="50" s="1" customFormat="1" ht="16" customHeight="1" spans="1:15">
+    <row r="50" s="1" customFormat="1" ht="17" customHeight="1" spans="1:15">
       <c r="A50" s="20"/>
-      <c r="B50" s="31" t="s">
-        <v>827</v>
-      </c>
-      <c r="C50" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="D50" s="28" t="s">
-        <v>493</v>
-      </c>
-      <c r="E50" s="28" t="s">
-        <v>828</v>
-      </c>
-      <c r="F50" s="29" t="s">
-        <v>829</v>
+      <c r="B50" s="31"/>
+      <c r="C50" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="E50" s="33" t="s">
+        <v>779</v>
+      </c>
+      <c r="F50" s="28" t="s">
+        <v>780</v>
       </c>
       <c r="G50" s="28"/>
       <c r="H50" s="28"/>
       <c r="I50" s="28"/>
-      <c r="J50" s="54"/>
+      <c r="J50" s="55"/>
       <c r="K50" s="23"/>
       <c r="L50" s="24"/>
       <c r="M50" s="22"/>
@@ -11284,58 +11290,78 @@
     <row r="51" s="1" customFormat="1" ht="22" customHeight="1" spans="1:15">
       <c r="A51" s="20"/>
       <c r="B51" s="31" t="s">
-        <v>830</v>
+        <v>781</v>
       </c>
       <c r="C51" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="D51" s="33" t="s">
-        <v>530</v>
-      </c>
-      <c r="E51" s="29" t="s">
-        <v>829</v>
-      </c>
-      <c r="F51" s="29" t="s">
-        <v>831</v>
+        <v>20</v>
+      </c>
+      <c r="D51" s="35" t="s">
+        <v>302</v>
+      </c>
+      <c r="E51" s="33" t="s">
+        <v>775</v>
+      </c>
+      <c r="F51" s="34" t="s">
+        <v>782</v>
       </c>
       <c r="G51" s="28"/>
       <c r="H51" s="28"/>
       <c r="I51" s="28"/>
-      <c r="J51" s="54"/>
+      <c r="J51" s="55"/>
       <c r="K51" s="23"/>
       <c r="L51" s="24"/>
       <c r="M51" s="22"/>
       <c r="N51" s="24"/>
       <c r="O51" s="23"/>
     </row>
-    <row r="52" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="52" s="1" customFormat="1" ht="16" customHeight="1" spans="1:15">
       <c r="A52" s="20"/>
-      <c r="B52" s="21"/>
-      <c r="C52" s="27"/>
-      <c r="D52" s="28"/>
-      <c r="E52" s="28"/>
-      <c r="F52" s="28"/>
+      <c r="B52" s="31" t="s">
+        <v>829</v>
+      </c>
+      <c r="C52" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D52" s="28" t="s">
+        <v>493</v>
+      </c>
+      <c r="E52" s="28" t="s">
+        <v>830</v>
+      </c>
+      <c r="F52" s="29" t="s">
+        <v>831</v>
+      </c>
       <c r="G52" s="28"/>
       <c r="H52" s="28"/>
       <c r="I52" s="28"/>
-      <c r="J52" s="54"/>
+      <c r="J52" s="55"/>
       <c r="K52" s="23"/>
       <c r="L52" s="24"/>
       <c r="M52" s="22"/>
       <c r="N52" s="24"/>
       <c r="O52" s="23"/>
     </row>
-    <row r="53" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+    <row r="53" s="1" customFormat="1" ht="22" customHeight="1" spans="1:15">
       <c r="A53" s="20"/>
-      <c r="B53" s="21"/>
-      <c r="C53" s="27"/>
-      <c r="D53" s="28"/>
-      <c r="E53" s="28"/>
-      <c r="F53" s="28"/>
+      <c r="B53" s="31" t="s">
+        <v>832</v>
+      </c>
+      <c r="C53" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="D53" s="33" t="s">
+        <v>530</v>
+      </c>
+      <c r="E53" s="29" t="s">
+        <v>831</v>
+      </c>
+      <c r="F53" s="29" t="s">
+        <v>833</v>
+      </c>
       <c r="G53" s="28"/>
       <c r="H53" s="28"/>
       <c r="I53" s="28"/>
-      <c r="J53" s="54"/>
+      <c r="J53" s="55"/>
       <c r="K53" s="23"/>
       <c r="L53" s="24"/>
       <c r="M53" s="22"/>
@@ -11352,7 +11378,7 @@
       <c r="G54" s="28"/>
       <c r="H54" s="28"/>
       <c r="I54" s="28"/>
-      <c r="J54" s="54"/>
+      <c r="J54" s="55"/>
       <c r="K54" s="23"/>
       <c r="L54" s="24"/>
       <c r="M54" s="22"/>
@@ -11369,7 +11395,7 @@
       <c r="G55" s="28"/>
       <c r="H55" s="28"/>
       <c r="I55" s="28"/>
-      <c r="J55" s="54"/>
+      <c r="J55" s="55"/>
       <c r="K55" s="23"/>
       <c r="L55" s="24"/>
       <c r="M55" s="22"/>
@@ -11386,7 +11412,7 @@
       <c r="G56" s="28"/>
       <c r="H56" s="28"/>
       <c r="I56" s="28"/>
-      <c r="J56" s="54"/>
+      <c r="J56" s="55"/>
       <c r="K56" s="23"/>
       <c r="L56" s="24"/>
       <c r="M56" s="22"/>
@@ -11403,7 +11429,7 @@
       <c r="G57" s="28"/>
       <c r="H57" s="28"/>
       <c r="I57" s="28"/>
-      <c r="J57" s="54"/>
+      <c r="J57" s="55"/>
       <c r="K57" s="23"/>
       <c r="L57" s="24"/>
       <c r="M57" s="22"/>
@@ -11420,7 +11446,7 @@
       <c r="G58" s="28"/>
       <c r="H58" s="28"/>
       <c r="I58" s="28"/>
-      <c r="J58" s="54"/>
+      <c r="J58" s="55"/>
       <c r="K58" s="23"/>
       <c r="L58" s="24"/>
       <c r="M58" s="22"/>
@@ -11437,7 +11463,7 @@
       <c r="G59" s="28"/>
       <c r="H59" s="28"/>
       <c r="I59" s="28"/>
-      <c r="J59" s="54"/>
+      <c r="J59" s="55"/>
       <c r="K59" s="23"/>
       <c r="L59" s="24"/>
       <c r="M59" s="22"/>
@@ -11454,7 +11480,7 @@
       <c r="G60" s="28"/>
       <c r="H60" s="28"/>
       <c r="I60" s="28"/>
-      <c r="J60" s="54"/>
+      <c r="J60" s="55"/>
       <c r="K60" s="23"/>
       <c r="L60" s="24"/>
       <c r="M60" s="22"/>
@@ -11471,7 +11497,7 @@
       <c r="G61" s="28"/>
       <c r="H61" s="28"/>
       <c r="I61" s="28"/>
-      <c r="J61" s="54"/>
+      <c r="J61" s="55"/>
       <c r="K61" s="23"/>
       <c r="L61" s="24"/>
       <c r="M61" s="22"/>
@@ -11488,7 +11514,7 @@
       <c r="G62" s="28"/>
       <c r="H62" s="28"/>
       <c r="I62" s="28"/>
-      <c r="J62" s="54"/>
+      <c r="J62" s="55"/>
       <c r="K62" s="23"/>
       <c r="L62" s="24"/>
       <c r="M62" s="22"/>
@@ -11505,7 +11531,7 @@
       <c r="G63" s="28"/>
       <c r="H63" s="28"/>
       <c r="I63" s="28"/>
-      <c r="J63" s="54"/>
+      <c r="J63" s="55"/>
       <c r="K63" s="23"/>
       <c r="L63" s="24"/>
       <c r="M63" s="22"/>
@@ -11522,7 +11548,7 @@
       <c r="G64" s="28"/>
       <c r="H64" s="28"/>
       <c r="I64" s="28"/>
-      <c r="J64" s="54"/>
+      <c r="J64" s="55"/>
       <c r="K64" s="23"/>
       <c r="L64" s="24"/>
       <c r="M64" s="22"/>
@@ -11539,7 +11565,7 @@
       <c r="G65" s="28"/>
       <c r="H65" s="28"/>
       <c r="I65" s="28"/>
-      <c r="J65" s="54"/>
+      <c r="J65" s="55"/>
       <c r="K65" s="23"/>
       <c r="L65" s="24"/>
       <c r="M65" s="22"/>
@@ -11556,7 +11582,7 @@
       <c r="G66" s="28"/>
       <c r="H66" s="28"/>
       <c r="I66" s="28"/>
-      <c r="J66" s="54"/>
+      <c r="J66" s="55"/>
       <c r="K66" s="23"/>
       <c r="L66" s="24"/>
       <c r="M66" s="22"/>
@@ -11573,7 +11599,7 @@
       <c r="G67" s="28"/>
       <c r="H67" s="28"/>
       <c r="I67" s="28"/>
-      <c r="J67" s="54"/>
+      <c r="J67" s="55"/>
       <c r="K67" s="23"/>
       <c r="L67" s="24"/>
       <c r="M67" s="22"/>
@@ -11590,7 +11616,7 @@
       <c r="G68" s="28"/>
       <c r="H68" s="28"/>
       <c r="I68" s="28"/>
-      <c r="J68" s="54"/>
+      <c r="J68" s="55"/>
       <c r="K68" s="23"/>
       <c r="L68" s="24"/>
       <c r="M68" s="22"/>
@@ -11607,7 +11633,7 @@
       <c r="G69" s="28"/>
       <c r="H69" s="28"/>
       <c r="I69" s="28"/>
-      <c r="J69" s="54"/>
+      <c r="J69" s="55"/>
       <c r="K69" s="23"/>
       <c r="L69" s="24"/>
       <c r="M69" s="22"/>
@@ -11624,7 +11650,7 @@
       <c r="G70" s="28"/>
       <c r="H70" s="28"/>
       <c r="I70" s="28"/>
-      <c r="J70" s="54"/>
+      <c r="J70" s="55"/>
       <c r="K70" s="23"/>
       <c r="L70" s="24"/>
       <c r="M70" s="22"/>
@@ -11641,7 +11667,7 @@
       <c r="G71" s="28"/>
       <c r="H71" s="28"/>
       <c r="I71" s="28"/>
-      <c r="J71" s="54"/>
+      <c r="J71" s="55"/>
       <c r="K71" s="23"/>
       <c r="L71" s="24"/>
       <c r="M71" s="22"/>
@@ -11658,7 +11684,7 @@
       <c r="G72" s="28"/>
       <c r="H72" s="28"/>
       <c r="I72" s="28"/>
-      <c r="J72" s="54"/>
+      <c r="J72" s="55"/>
       <c r="K72" s="23"/>
       <c r="L72" s="24"/>
       <c r="M72" s="22"/>
@@ -11675,7 +11701,7 @@
       <c r="G73" s="28"/>
       <c r="H73" s="28"/>
       <c r="I73" s="28"/>
-      <c r="J73" s="54"/>
+      <c r="J73" s="55"/>
       <c r="K73" s="23"/>
       <c r="L73" s="24"/>
       <c r="M73" s="22"/>
@@ -11692,7 +11718,7 @@
       <c r="G74" s="28"/>
       <c r="H74" s="28"/>
       <c r="I74" s="28"/>
-      <c r="J74" s="54"/>
+      <c r="J74" s="55"/>
       <c r="K74" s="23"/>
       <c r="L74" s="24"/>
       <c r="M74" s="22"/>
@@ -11709,7 +11735,7 @@
       <c r="G75" s="28"/>
       <c r="H75" s="28"/>
       <c r="I75" s="28"/>
-      <c r="J75" s="54"/>
+      <c r="J75" s="55"/>
       <c r="K75" s="23"/>
       <c r="L75" s="24"/>
       <c r="M75" s="22"/>
@@ -11726,7 +11752,7 @@
       <c r="G76" s="28"/>
       <c r="H76" s="28"/>
       <c r="I76" s="28"/>
-      <c r="J76" s="54"/>
+      <c r="J76" s="55"/>
       <c r="K76" s="23"/>
       <c r="L76" s="24"/>
       <c r="M76" s="22"/>
@@ -11743,7 +11769,7 @@
       <c r="G77" s="28"/>
       <c r="H77" s="28"/>
       <c r="I77" s="28"/>
-      <c r="J77" s="54"/>
+      <c r="J77" s="55"/>
       <c r="K77" s="23"/>
       <c r="L77" s="24"/>
       <c r="M77" s="22"/>
@@ -11760,7 +11786,7 @@
       <c r="G78" s="28"/>
       <c r="H78" s="28"/>
       <c r="I78" s="28"/>
-      <c r="J78" s="54"/>
+      <c r="J78" s="55"/>
       <c r="K78" s="23"/>
       <c r="L78" s="24"/>
       <c r="M78" s="22"/>
@@ -11777,7 +11803,7 @@
       <c r="G79" s="28"/>
       <c r="H79" s="28"/>
       <c r="I79" s="28"/>
-      <c r="J79" s="54"/>
+      <c r="J79" s="55"/>
       <c r="K79" s="23"/>
       <c r="L79" s="24"/>
       <c r="M79" s="22"/>
@@ -11794,7 +11820,7 @@
       <c r="G80" s="28"/>
       <c r="H80" s="28"/>
       <c r="I80" s="28"/>
-      <c r="J80" s="54"/>
+      <c r="J80" s="55"/>
       <c r="K80" s="23"/>
       <c r="L80" s="24"/>
       <c r="M80" s="22"/>
@@ -11811,7 +11837,7 @@
       <c r="G81" s="28"/>
       <c r="H81" s="28"/>
       <c r="I81" s="28"/>
-      <c r="J81" s="54"/>
+      <c r="J81" s="55"/>
       <c r="K81" s="23"/>
       <c r="L81" s="24"/>
       <c r="M81" s="22"/>
@@ -11828,7 +11854,7 @@
       <c r="G82" s="28"/>
       <c r="H82" s="28"/>
       <c r="I82" s="28"/>
-      <c r="J82" s="54"/>
+      <c r="J82" s="55"/>
       <c r="K82" s="23"/>
       <c r="L82" s="24"/>
       <c r="M82" s="22"/>
@@ -11845,7 +11871,7 @@
       <c r="G83" s="28"/>
       <c r="H83" s="28"/>
       <c r="I83" s="28"/>
-      <c r="J83" s="54"/>
+      <c r="J83" s="55"/>
       <c r="K83" s="23"/>
       <c r="L83" s="24"/>
       <c r="M83" s="22"/>
@@ -11862,7 +11888,7 @@
       <c r="G84" s="28"/>
       <c r="H84" s="28"/>
       <c r="I84" s="28"/>
-      <c r="J84" s="54"/>
+      <c r="J84" s="55"/>
       <c r="K84" s="23"/>
       <c r="L84" s="24"/>
       <c r="M84" s="22"/>
@@ -11879,7 +11905,7 @@
       <c r="G85" s="28"/>
       <c r="H85" s="28"/>
       <c r="I85" s="28"/>
-      <c r="J85" s="54"/>
+      <c r="J85" s="55"/>
       <c r="K85" s="23"/>
       <c r="L85" s="24"/>
       <c r="M85" s="22"/>
@@ -11896,7 +11922,7 @@
       <c r="G86" s="28"/>
       <c r="H86" s="28"/>
       <c r="I86" s="28"/>
-      <c r="J86" s="54"/>
+      <c r="J86" s="55"/>
       <c r="K86" s="23"/>
       <c r="L86" s="24"/>
       <c r="M86" s="22"/>
@@ -11913,7 +11939,7 @@
       <c r="G87" s="28"/>
       <c r="H87" s="28"/>
       <c r="I87" s="28"/>
-      <c r="J87" s="54"/>
+      <c r="J87" s="55"/>
       <c r="K87" s="23"/>
       <c r="L87" s="24"/>
       <c r="M87" s="22"/>
@@ -11930,7 +11956,7 @@
       <c r="G88" s="28"/>
       <c r="H88" s="28"/>
       <c r="I88" s="28"/>
-      <c r="J88" s="54"/>
+      <c r="J88" s="55"/>
       <c r="K88" s="23"/>
       <c r="L88" s="24"/>
       <c r="M88" s="22"/>
@@ -11947,7 +11973,7 @@
       <c r="G89" s="28"/>
       <c r="H89" s="28"/>
       <c r="I89" s="28"/>
-      <c r="J89" s="54"/>
+      <c r="J89" s="55"/>
       <c r="K89" s="23"/>
       <c r="L89" s="24"/>
       <c r="M89" s="22"/>
@@ -11964,7 +11990,7 @@
       <c r="G90" s="28"/>
       <c r="H90" s="28"/>
       <c r="I90" s="28"/>
-      <c r="J90" s="54"/>
+      <c r="J90" s="55"/>
       <c r="K90" s="23"/>
       <c r="L90" s="24"/>
       <c r="M90" s="22"/>
@@ -11981,7 +12007,7 @@
       <c r="G91" s="28"/>
       <c r="H91" s="28"/>
       <c r="I91" s="28"/>
-      <c r="J91" s="54"/>
+      <c r="J91" s="55"/>
       <c r="K91" s="23"/>
       <c r="L91" s="24"/>
       <c r="M91" s="22"/>
@@ -11998,7 +12024,7 @@
       <c r="G92" s="28"/>
       <c r="H92" s="28"/>
       <c r="I92" s="28"/>
-      <c r="J92" s="54"/>
+      <c r="J92" s="55"/>
       <c r="K92" s="23"/>
       <c r="L92" s="24"/>
       <c r="M92" s="22"/>
@@ -12015,7 +12041,7 @@
       <c r="G93" s="28"/>
       <c r="H93" s="28"/>
       <c r="I93" s="28"/>
-      <c r="J93" s="54"/>
+      <c r="J93" s="55"/>
       <c r="K93" s="23"/>
       <c r="L93" s="24"/>
       <c r="M93" s="22"/>
@@ -12032,7 +12058,7 @@
       <c r="G94" s="28"/>
       <c r="H94" s="28"/>
       <c r="I94" s="28"/>
-      <c r="J94" s="54"/>
+      <c r="J94" s="55"/>
       <c r="K94" s="23"/>
       <c r="L94" s="24"/>
       <c r="M94" s="22"/>
@@ -12049,7 +12075,7 @@
       <c r="G95" s="28"/>
       <c r="H95" s="28"/>
       <c r="I95" s="28"/>
-      <c r="J95" s="54"/>
+      <c r="J95" s="55"/>
       <c r="K95" s="23"/>
       <c r="L95" s="24"/>
       <c r="M95" s="22"/>
@@ -12066,7 +12092,7 @@
       <c r="G96" s="28"/>
       <c r="H96" s="28"/>
       <c r="I96" s="28"/>
-      <c r="J96" s="54"/>
+      <c r="J96" s="55"/>
       <c r="K96" s="23"/>
       <c r="L96" s="24"/>
       <c r="M96" s="22"/>
@@ -12083,7 +12109,7 @@
       <c r="G97" s="28"/>
       <c r="H97" s="28"/>
       <c r="I97" s="28"/>
-      <c r="J97" s="54"/>
+      <c r="J97" s="55"/>
       <c r="K97" s="23"/>
       <c r="L97" s="24"/>
       <c r="M97" s="22"/>
@@ -12100,7 +12126,7 @@
       <c r="G98" s="28"/>
       <c r="H98" s="28"/>
       <c r="I98" s="28"/>
-      <c r="J98" s="54"/>
+      <c r="J98" s="55"/>
       <c r="K98" s="23"/>
       <c r="L98" s="24"/>
       <c r="M98" s="22"/>
@@ -12117,7 +12143,7 @@
       <c r="G99" s="28"/>
       <c r="H99" s="28"/>
       <c r="I99" s="28"/>
-      <c r="J99" s="54"/>
+      <c r="J99" s="55"/>
       <c r="K99" s="23"/>
       <c r="L99" s="24"/>
       <c r="M99" s="22"/>
@@ -12134,7 +12160,7 @@
       <c r="G100" s="28"/>
       <c r="H100" s="28"/>
       <c r="I100" s="28"/>
-      <c r="J100" s="54"/>
+      <c r="J100" s="55"/>
       <c r="K100" s="23"/>
       <c r="L100" s="24"/>
       <c r="M100" s="22"/>
@@ -12151,7 +12177,7 @@
       <c r="G101" s="28"/>
       <c r="H101" s="28"/>
       <c r="I101" s="28"/>
-      <c r="J101" s="54"/>
+      <c r="J101" s="55"/>
       <c r="K101" s="23"/>
       <c r="L101" s="24"/>
       <c r="M101" s="22"/>
@@ -12168,7 +12194,7 @@
       <c r="G102" s="28"/>
       <c r="H102" s="28"/>
       <c r="I102" s="28"/>
-      <c r="J102" s="54"/>
+      <c r="J102" s="55"/>
       <c r="K102" s="23"/>
       <c r="L102" s="24"/>
       <c r="M102" s="22"/>
@@ -12185,7 +12211,7 @@
       <c r="G103" s="28"/>
       <c r="H103" s="28"/>
       <c r="I103" s="28"/>
-      <c r="J103" s="54"/>
+      <c r="J103" s="55"/>
       <c r="K103" s="23"/>
       <c r="L103" s="24"/>
       <c r="M103" s="22"/>
@@ -12202,7 +12228,7 @@
       <c r="G104" s="28"/>
       <c r="H104" s="28"/>
       <c r="I104" s="28"/>
-      <c r="J104" s="54"/>
+      <c r="J104" s="55"/>
       <c r="K104" s="23"/>
       <c r="L104" s="24"/>
       <c r="M104" s="22"/>
@@ -12219,7 +12245,7 @@
       <c r="G105" s="28"/>
       <c r="H105" s="28"/>
       <c r="I105" s="28"/>
-      <c r="J105" s="54"/>
+      <c r="J105" s="55"/>
       <c r="K105" s="23"/>
       <c r="L105" s="24"/>
       <c r="M105" s="22"/>
@@ -12236,7 +12262,7 @@
       <c r="G106" s="28"/>
       <c r="H106" s="28"/>
       <c r="I106" s="28"/>
-      <c r="J106" s="54"/>
+      <c r="J106" s="55"/>
       <c r="K106" s="23"/>
       <c r="L106" s="24"/>
       <c r="M106" s="22"/>
@@ -12253,7 +12279,7 @@
       <c r="G107" s="28"/>
       <c r="H107" s="28"/>
       <c r="I107" s="28"/>
-      <c r="J107" s="54"/>
+      <c r="J107" s="55"/>
       <c r="K107" s="23"/>
       <c r="L107" s="24"/>
       <c r="M107" s="22"/>
@@ -12270,7 +12296,7 @@
       <c r="G108" s="28"/>
       <c r="H108" s="28"/>
       <c r="I108" s="28"/>
-      <c r="J108" s="54"/>
+      <c r="J108" s="55"/>
       <c r="K108" s="23"/>
       <c r="L108" s="24"/>
       <c r="M108" s="22"/>
@@ -12287,7 +12313,7 @@
       <c r="G109" s="28"/>
       <c r="H109" s="28"/>
       <c r="I109" s="28"/>
-      <c r="J109" s="54"/>
+      <c r="J109" s="55"/>
       <c r="K109" s="23"/>
       <c r="L109" s="24"/>
       <c r="M109" s="22"/>
@@ -12304,7 +12330,7 @@
       <c r="G110" s="28"/>
       <c r="H110" s="28"/>
       <c r="I110" s="28"/>
-      <c r="J110" s="54"/>
+      <c r="J110" s="55"/>
       <c r="K110" s="23"/>
       <c r="L110" s="24"/>
       <c r="M110" s="22"/>
@@ -12321,7 +12347,7 @@
       <c r="G111" s="28"/>
       <c r="H111" s="28"/>
       <c r="I111" s="28"/>
-      <c r="J111" s="54"/>
+      <c r="J111" s="55"/>
       <c r="K111" s="23"/>
       <c r="L111" s="24"/>
       <c r="M111" s="22"/>
@@ -12338,7 +12364,7 @@
       <c r="G112" s="28"/>
       <c r="H112" s="28"/>
       <c r="I112" s="28"/>
-      <c r="J112" s="54"/>
+      <c r="J112" s="55"/>
       <c r="K112" s="23"/>
       <c r="L112" s="24"/>
       <c r="M112" s="22"/>
@@ -12355,7 +12381,7 @@
       <c r="G113" s="28"/>
       <c r="H113" s="28"/>
       <c r="I113" s="28"/>
-      <c r="J113" s="54"/>
+      <c r="J113" s="55"/>
       <c r="K113" s="23"/>
       <c r="L113" s="24"/>
       <c r="M113" s="22"/>
@@ -12372,7 +12398,7 @@
       <c r="G114" s="28"/>
       <c r="H114" s="28"/>
       <c r="I114" s="28"/>
-      <c r="J114" s="54"/>
+      <c r="J114" s="55"/>
       <c r="K114" s="23"/>
       <c r="L114" s="24"/>
       <c r="M114" s="22"/>
@@ -12389,7 +12415,7 @@
       <c r="G115" s="28"/>
       <c r="H115" s="28"/>
       <c r="I115" s="28"/>
-      <c r="J115" s="54"/>
+      <c r="J115" s="55"/>
       <c r="K115" s="23"/>
       <c r="L115" s="24"/>
       <c r="M115" s="22"/>
@@ -12406,7 +12432,7 @@
       <c r="G116" s="28"/>
       <c r="H116" s="28"/>
       <c r="I116" s="28"/>
-      <c r="J116" s="54"/>
+      <c r="J116" s="55"/>
       <c r="K116" s="23"/>
       <c r="L116" s="24"/>
       <c r="M116" s="22"/>
@@ -12423,7 +12449,7 @@
       <c r="G117" s="28"/>
       <c r="H117" s="28"/>
       <c r="I117" s="28"/>
-      <c r="J117" s="54"/>
+      <c r="J117" s="55"/>
       <c r="K117" s="23"/>
       <c r="L117" s="24"/>
       <c r="M117" s="22"/>
@@ -12440,7 +12466,7 @@
       <c r="G118" s="28"/>
       <c r="H118" s="28"/>
       <c r="I118" s="28"/>
-      <c r="J118" s="54"/>
+      <c r="J118" s="55"/>
       <c r="K118" s="23"/>
       <c r="L118" s="24"/>
       <c r="M118" s="22"/>
@@ -12457,7 +12483,7 @@
       <c r="G119" s="28"/>
       <c r="H119" s="28"/>
       <c r="I119" s="28"/>
-      <c r="J119" s="54"/>
+      <c r="J119" s="55"/>
       <c r="K119" s="23"/>
       <c r="L119" s="24"/>
       <c r="M119" s="22"/>
@@ -12474,7 +12500,7 @@
       <c r="G120" s="28"/>
       <c r="H120" s="28"/>
       <c r="I120" s="28"/>
-      <c r="J120" s="54"/>
+      <c r="J120" s="55"/>
       <c r="K120" s="23"/>
       <c r="L120" s="24"/>
       <c r="M120" s="22"/>
@@ -12491,7 +12517,7 @@
       <c r="G121" s="28"/>
       <c r="H121" s="28"/>
       <c r="I121" s="28"/>
-      <c r="J121" s="54"/>
+      <c r="J121" s="55"/>
       <c r="K121" s="23"/>
       <c r="L121" s="24"/>
       <c r="M121" s="22"/>
@@ -12508,7 +12534,7 @@
       <c r="G122" s="28"/>
       <c r="H122" s="28"/>
       <c r="I122" s="28"/>
-      <c r="J122" s="54"/>
+      <c r="J122" s="55"/>
       <c r="K122" s="23"/>
       <c r="L122" s="24"/>
       <c r="M122" s="22"/>
@@ -12525,7 +12551,7 @@
       <c r="G123" s="28"/>
       <c r="H123" s="28"/>
       <c r="I123" s="28"/>
-      <c r="J123" s="54"/>
+      <c r="J123" s="55"/>
       <c r="K123" s="23"/>
       <c r="L123" s="24"/>
       <c r="M123" s="22"/>
@@ -12542,7 +12568,7 @@
       <c r="G124" s="28"/>
       <c r="H124" s="28"/>
       <c r="I124" s="28"/>
-      <c r="J124" s="54"/>
+      <c r="J124" s="55"/>
       <c r="K124" s="23"/>
       <c r="L124" s="24"/>
       <c r="M124" s="22"/>
@@ -12559,7 +12585,7 @@
       <c r="G125" s="28"/>
       <c r="H125" s="28"/>
       <c r="I125" s="28"/>
-      <c r="J125" s="54"/>
+      <c r="J125" s="55"/>
       <c r="K125" s="23"/>
       <c r="L125" s="24"/>
       <c r="M125" s="22"/>
@@ -12576,7 +12602,7 @@
       <c r="G126" s="28"/>
       <c r="H126" s="28"/>
       <c r="I126" s="28"/>
-      <c r="J126" s="54"/>
+      <c r="J126" s="55"/>
       <c r="K126" s="23"/>
       <c r="L126" s="24"/>
       <c r="M126" s="22"/>
@@ -12593,7 +12619,7 @@
       <c r="G127" s="28"/>
       <c r="H127" s="28"/>
       <c r="I127" s="28"/>
-      <c r="J127" s="54"/>
+      <c r="J127" s="55"/>
       <c r="K127" s="23"/>
       <c r="L127" s="24"/>
       <c r="M127" s="22"/>
@@ -12610,7 +12636,7 @@
       <c r="G128" s="28"/>
       <c r="H128" s="28"/>
       <c r="I128" s="28"/>
-      <c r="J128" s="54"/>
+      <c r="J128" s="55"/>
       <c r="K128" s="23"/>
       <c r="L128" s="24"/>
       <c r="M128" s="22"/>
@@ -12627,7 +12653,7 @@
       <c r="G129" s="28"/>
       <c r="H129" s="28"/>
       <c r="I129" s="28"/>
-      <c r="J129" s="54"/>
+      <c r="J129" s="55"/>
       <c r="K129" s="23"/>
       <c r="L129" s="24"/>
       <c r="M129" s="22"/>
@@ -12644,7 +12670,7 @@
       <c r="G130" s="28"/>
       <c r="H130" s="28"/>
       <c r="I130" s="28"/>
-      <c r="J130" s="54"/>
+      <c r="J130" s="55"/>
       <c r="K130" s="23"/>
       <c r="L130" s="24"/>
       <c r="M130" s="22"/>
@@ -12661,7 +12687,7 @@
       <c r="G131" s="28"/>
       <c r="H131" s="28"/>
       <c r="I131" s="28"/>
-      <c r="J131" s="54"/>
+      <c r="J131" s="55"/>
       <c r="K131" s="23"/>
       <c r="L131" s="24"/>
       <c r="M131" s="22"/>
@@ -12678,7 +12704,7 @@
       <c r="G132" s="28"/>
       <c r="H132" s="28"/>
       <c r="I132" s="28"/>
-      <c r="J132" s="54"/>
+      <c r="J132" s="55"/>
       <c r="K132" s="23"/>
       <c r="L132" s="24"/>
       <c r="M132" s="22"/>
@@ -12695,7 +12721,7 @@
       <c r="G133" s="28"/>
       <c r="H133" s="28"/>
       <c r="I133" s="28"/>
-      <c r="J133" s="54"/>
+      <c r="J133" s="55"/>
       <c r="K133" s="23"/>
       <c r="L133" s="24"/>
       <c r="M133" s="22"/>
@@ -12712,7 +12738,7 @@
       <c r="G134" s="28"/>
       <c r="H134" s="28"/>
       <c r="I134" s="28"/>
-      <c r="J134" s="54"/>
+      <c r="J134" s="55"/>
       <c r="K134" s="23"/>
       <c r="L134" s="24"/>
       <c r="M134" s="22"/>
@@ -12729,7 +12755,7 @@
       <c r="G135" s="28"/>
       <c r="H135" s="28"/>
       <c r="I135" s="28"/>
-      <c r="J135" s="54"/>
+      <c r="J135" s="55"/>
       <c r="K135" s="23"/>
       <c r="L135" s="24"/>
       <c r="M135" s="22"/>
@@ -12746,7 +12772,7 @@
       <c r="G136" s="28"/>
       <c r="H136" s="28"/>
       <c r="I136" s="28"/>
-      <c r="J136" s="54"/>
+      <c r="J136" s="55"/>
       <c r="K136" s="23"/>
       <c r="L136" s="24"/>
       <c r="M136" s="22"/>
@@ -12763,7 +12789,7 @@
       <c r="G137" s="28"/>
       <c r="H137" s="28"/>
       <c r="I137" s="28"/>
-      <c r="J137" s="54"/>
+      <c r="J137" s="55"/>
       <c r="K137" s="23"/>
       <c r="L137" s="24"/>
       <c r="M137" s="22"/>
@@ -12780,7 +12806,7 @@
       <c r="G138" s="28"/>
       <c r="H138" s="28"/>
       <c r="I138" s="28"/>
-      <c r="J138" s="54"/>
+      <c r="J138" s="55"/>
       <c r="K138" s="23"/>
       <c r="L138" s="24"/>
       <c r="M138" s="22"/>
@@ -12797,7 +12823,7 @@
       <c r="G139" s="28"/>
       <c r="H139" s="28"/>
       <c r="I139" s="28"/>
-      <c r="J139" s="54"/>
+      <c r="J139" s="55"/>
       <c r="K139" s="23"/>
       <c r="L139" s="24"/>
       <c r="M139" s="22"/>
@@ -12814,7 +12840,7 @@
       <c r="G140" s="28"/>
       <c r="H140" s="28"/>
       <c r="I140" s="28"/>
-      <c r="J140" s="54"/>
+      <c r="J140" s="55"/>
       <c r="K140" s="23"/>
       <c r="L140" s="24"/>
       <c r="M140" s="22"/>
@@ -12831,7 +12857,7 @@
       <c r="G141" s="28"/>
       <c r="H141" s="28"/>
       <c r="I141" s="28"/>
-      <c r="J141" s="54"/>
+      <c r="J141" s="55"/>
       <c r="K141" s="23"/>
       <c r="L141" s="24"/>
       <c r="M141" s="22"/>
@@ -12848,7 +12874,7 @@
       <c r="G142" s="28"/>
       <c r="H142" s="28"/>
       <c r="I142" s="28"/>
-      <c r="J142" s="54"/>
+      <c r="J142" s="55"/>
       <c r="K142" s="23"/>
       <c r="L142" s="24"/>
       <c r="M142" s="22"/>
@@ -12865,7 +12891,7 @@
       <c r="G143" s="28"/>
       <c r="H143" s="28"/>
       <c r="I143" s="28"/>
-      <c r="J143" s="54"/>
+      <c r="J143" s="55"/>
       <c r="K143" s="23"/>
       <c r="L143" s="24"/>
       <c r="M143" s="22"/>
@@ -12882,7 +12908,7 @@
       <c r="G144" s="28"/>
       <c r="H144" s="28"/>
       <c r="I144" s="28"/>
-      <c r="J144" s="54"/>
+      <c r="J144" s="55"/>
       <c r="K144" s="23"/>
       <c r="L144" s="24"/>
       <c r="M144" s="22"/>
@@ -12899,7 +12925,7 @@
       <c r="G145" s="28"/>
       <c r="H145" s="28"/>
       <c r="I145" s="28"/>
-      <c r="J145" s="54"/>
+      <c r="J145" s="55"/>
       <c r="K145" s="23"/>
       <c r="L145" s="24"/>
       <c r="M145" s="22"/>
@@ -12916,7 +12942,7 @@
       <c r="G146" s="28"/>
       <c r="H146" s="28"/>
       <c r="I146" s="28"/>
-      <c r="J146" s="54"/>
+      <c r="J146" s="55"/>
       <c r="K146" s="23"/>
       <c r="L146" s="24"/>
       <c r="M146" s="22"/>
@@ -12933,7 +12959,7 @@
       <c r="G147" s="28"/>
       <c r="H147" s="28"/>
       <c r="I147" s="28"/>
-      <c r="J147" s="54"/>
+      <c r="J147" s="55"/>
       <c r="K147" s="23"/>
       <c r="L147" s="24"/>
       <c r="M147" s="22"/>
@@ -12950,7 +12976,7 @@
       <c r="G148" s="28"/>
       <c r="H148" s="28"/>
       <c r="I148" s="28"/>
-      <c r="J148" s="54"/>
+      <c r="J148" s="55"/>
       <c r="K148" s="23"/>
       <c r="L148" s="24"/>
       <c r="M148" s="22"/>
@@ -12967,7 +12993,7 @@
       <c r="G149" s="28"/>
       <c r="H149" s="28"/>
       <c r="I149" s="28"/>
-      <c r="J149" s="54"/>
+      <c r="J149" s="55"/>
       <c r="K149" s="23"/>
       <c r="L149" s="24"/>
       <c r="M149" s="22"/>
@@ -12984,7 +13010,7 @@
       <c r="G150" s="28"/>
       <c r="H150" s="28"/>
       <c r="I150" s="28"/>
-      <c r="J150" s="54"/>
+      <c r="J150" s="55"/>
       <c r="K150" s="23"/>
       <c r="L150" s="24"/>
       <c r="M150" s="22"/>
@@ -13001,7 +13027,7 @@
       <c r="G151" s="28"/>
       <c r="H151" s="28"/>
       <c r="I151" s="28"/>
-      <c r="J151" s="54"/>
+      <c r="J151" s="55"/>
       <c r="K151" s="23"/>
       <c r="L151" s="24"/>
       <c r="M151" s="22"/>
@@ -13018,7 +13044,7 @@
       <c r="G152" s="28"/>
       <c r="H152" s="28"/>
       <c r="I152" s="28"/>
-      <c r="J152" s="54"/>
+      <c r="J152" s="55"/>
       <c r="K152" s="23"/>
       <c r="L152" s="24"/>
       <c r="M152" s="22"/>
@@ -13035,7 +13061,7 @@
       <c r="G153" s="28"/>
       <c r="H153" s="28"/>
       <c r="I153" s="28"/>
-      <c r="J153" s="54"/>
+      <c r="J153" s="55"/>
       <c r="K153" s="23"/>
       <c r="L153" s="24"/>
       <c r="M153" s="22"/>
@@ -13052,7 +13078,7 @@
       <c r="G154" s="28"/>
       <c r="H154" s="28"/>
       <c r="I154" s="28"/>
-      <c r="J154" s="54"/>
+      <c r="J154" s="55"/>
       <c r="K154" s="23"/>
       <c r="L154" s="24"/>
       <c r="M154" s="22"/>
@@ -13069,7 +13095,7 @@
       <c r="G155" s="28"/>
       <c r="H155" s="28"/>
       <c r="I155" s="28"/>
-      <c r="J155" s="54"/>
+      <c r="J155" s="55"/>
       <c r="K155" s="23"/>
       <c r="L155" s="24"/>
       <c r="M155" s="22"/>
@@ -13086,7 +13112,7 @@
       <c r="G156" s="28"/>
       <c r="H156" s="28"/>
       <c r="I156" s="28"/>
-      <c r="J156" s="54"/>
+      <c r="J156" s="55"/>
       <c r="K156" s="23"/>
       <c r="L156" s="24"/>
       <c r="M156" s="22"/>
@@ -13103,7 +13129,7 @@
       <c r="G157" s="28"/>
       <c r="H157" s="28"/>
       <c r="I157" s="28"/>
-      <c r="J157" s="54"/>
+      <c r="J157" s="55"/>
       <c r="K157" s="23"/>
       <c r="L157" s="24"/>
       <c r="M157" s="22"/>
@@ -13120,7 +13146,7 @@
       <c r="G158" s="28"/>
       <c r="H158" s="28"/>
       <c r="I158" s="28"/>
-      <c r="J158" s="54"/>
+      <c r="J158" s="55"/>
       <c r="K158" s="23"/>
       <c r="L158" s="24"/>
       <c r="M158" s="22"/>
@@ -13137,7 +13163,7 @@
       <c r="G159" s="28"/>
       <c r="H159" s="28"/>
       <c r="I159" s="28"/>
-      <c r="J159" s="54"/>
+      <c r="J159" s="55"/>
       <c r="K159" s="23"/>
       <c r="L159" s="24"/>
       <c r="M159" s="22"/>
@@ -13154,7 +13180,7 @@
       <c r="G160" s="28"/>
       <c r="H160" s="28"/>
       <c r="I160" s="28"/>
-      <c r="J160" s="54"/>
+      <c r="J160" s="55"/>
       <c r="K160" s="23"/>
       <c r="L160" s="24"/>
       <c r="M160" s="22"/>
@@ -13171,7 +13197,7 @@
       <c r="G161" s="28"/>
       <c r="H161" s="28"/>
       <c r="I161" s="28"/>
-      <c r="J161" s="54"/>
+      <c r="J161" s="55"/>
       <c r="K161" s="23"/>
       <c r="L161" s="24"/>
       <c r="M161" s="22"/>
@@ -13188,7 +13214,7 @@
       <c r="G162" s="28"/>
       <c r="H162" s="28"/>
       <c r="I162" s="28"/>
-      <c r="J162" s="54"/>
+      <c r="J162" s="55"/>
       <c r="K162" s="23"/>
       <c r="L162" s="24"/>
       <c r="M162" s="22"/>
@@ -13205,7 +13231,7 @@
       <c r="G163" s="28"/>
       <c r="H163" s="28"/>
       <c r="I163" s="28"/>
-      <c r="J163" s="54"/>
+      <c r="J163" s="55"/>
       <c r="K163" s="23"/>
       <c r="L163" s="24"/>
       <c r="M163" s="22"/>
@@ -13222,7 +13248,7 @@
       <c r="G164" s="28"/>
       <c r="H164" s="28"/>
       <c r="I164" s="28"/>
-      <c r="J164" s="54"/>
+      <c r="J164" s="55"/>
       <c r="K164" s="23"/>
       <c r="L164" s="24"/>
       <c r="M164" s="22"/>
@@ -13239,7 +13265,7 @@
       <c r="G165" s="28"/>
       <c r="H165" s="28"/>
       <c r="I165" s="28"/>
-      <c r="J165" s="54"/>
+      <c r="J165" s="55"/>
       <c r="K165" s="23"/>
       <c r="L165" s="24"/>
       <c r="M165" s="22"/>
@@ -13256,7 +13282,7 @@
       <c r="G166" s="28"/>
       <c r="H166" s="28"/>
       <c r="I166" s="28"/>
-      <c r="J166" s="54"/>
+      <c r="J166" s="55"/>
       <c r="K166" s="23"/>
       <c r="L166" s="24"/>
       <c r="M166" s="22"/>
@@ -13273,7 +13299,7 @@
       <c r="G167" s="28"/>
       <c r="H167" s="28"/>
       <c r="I167" s="28"/>
-      <c r="J167" s="54"/>
+      <c r="J167" s="55"/>
       <c r="K167" s="23"/>
       <c r="L167" s="24"/>
       <c r="M167" s="22"/>
@@ -13290,7 +13316,7 @@
       <c r="G168" s="28"/>
       <c r="H168" s="28"/>
       <c r="I168" s="28"/>
-      <c r="J168" s="54"/>
+      <c r="J168" s="55"/>
       <c r="K168" s="23"/>
       <c r="L168" s="24"/>
       <c r="M168" s="22"/>
@@ -13307,7 +13333,7 @@
       <c r="G169" s="28"/>
       <c r="H169" s="28"/>
       <c r="I169" s="28"/>
-      <c r="J169" s="54"/>
+      <c r="J169" s="55"/>
       <c r="K169" s="23"/>
       <c r="L169" s="24"/>
       <c r="M169" s="22"/>
@@ -13324,7 +13350,7 @@
       <c r="G170" s="28"/>
       <c r="H170" s="28"/>
       <c r="I170" s="28"/>
-      <c r="J170" s="54"/>
+      <c r="J170" s="55"/>
       <c r="K170" s="23"/>
       <c r="L170" s="24"/>
       <c r="M170" s="22"/>
@@ -13341,7 +13367,7 @@
       <c r="G171" s="28"/>
       <c r="H171" s="28"/>
       <c r="I171" s="28"/>
-      <c r="J171" s="54"/>
+      <c r="J171" s="55"/>
       <c r="K171" s="23"/>
       <c r="L171" s="24"/>
       <c r="M171" s="22"/>
@@ -13358,7 +13384,7 @@
       <c r="G172" s="28"/>
       <c r="H172" s="28"/>
       <c r="I172" s="28"/>
-      <c r="J172" s="54"/>
+      <c r="J172" s="55"/>
       <c r="K172" s="23"/>
       <c r="L172" s="24"/>
       <c r="M172" s="22"/>
@@ -13375,7 +13401,7 @@
       <c r="G173" s="28"/>
       <c r="H173" s="28"/>
       <c r="I173" s="28"/>
-      <c r="J173" s="54"/>
+      <c r="J173" s="55"/>
       <c r="K173" s="23"/>
       <c r="L173" s="24"/>
       <c r="M173" s="22"/>
@@ -13392,7 +13418,7 @@
       <c r="G174" s="28"/>
       <c r="H174" s="28"/>
       <c r="I174" s="28"/>
-      <c r="J174" s="54"/>
+      <c r="J174" s="55"/>
       <c r="K174" s="23"/>
       <c r="L174" s="24"/>
       <c r="M174" s="22"/>
@@ -13409,7 +13435,7 @@
       <c r="G175" s="28"/>
       <c r="H175" s="28"/>
       <c r="I175" s="28"/>
-      <c r="J175" s="54"/>
+      <c r="J175" s="55"/>
       <c r="K175" s="23"/>
       <c r="L175" s="24"/>
       <c r="M175" s="22"/>
@@ -13426,7 +13452,7 @@
       <c r="G176" s="28"/>
       <c r="H176" s="28"/>
       <c r="I176" s="28"/>
-      <c r="J176" s="54"/>
+      <c r="J176" s="55"/>
       <c r="K176" s="23"/>
       <c r="L176" s="24"/>
       <c r="M176" s="22"/>
@@ -13443,7 +13469,7 @@
       <c r="G177" s="28"/>
       <c r="H177" s="28"/>
       <c r="I177" s="28"/>
-      <c r="J177" s="54"/>
+      <c r="J177" s="55"/>
       <c r="K177" s="23"/>
       <c r="L177" s="24"/>
       <c r="M177" s="22"/>
@@ -13460,7 +13486,7 @@
       <c r="G178" s="28"/>
       <c r="H178" s="28"/>
       <c r="I178" s="28"/>
-      <c r="J178" s="54"/>
+      <c r="J178" s="55"/>
       <c r="K178" s="23"/>
       <c r="L178" s="24"/>
       <c r="M178" s="22"/>
@@ -13477,7 +13503,7 @@
       <c r="G179" s="28"/>
       <c r="H179" s="28"/>
       <c r="I179" s="28"/>
-      <c r="J179" s="54"/>
+      <c r="J179" s="55"/>
       <c r="K179" s="23"/>
       <c r="L179" s="24"/>
       <c r="M179" s="22"/>
@@ -13494,7 +13520,7 @@
       <c r="G180" s="28"/>
       <c r="H180" s="28"/>
       <c r="I180" s="28"/>
-      <c r="J180" s="54"/>
+      <c r="J180" s="55"/>
       <c r="K180" s="23"/>
       <c r="L180" s="24"/>
       <c r="M180" s="22"/>
@@ -13511,7 +13537,7 @@
       <c r="G181" s="28"/>
       <c r="H181" s="28"/>
       <c r="I181" s="28"/>
-      <c r="J181" s="54"/>
+      <c r="J181" s="55"/>
       <c r="K181" s="23"/>
       <c r="L181" s="24"/>
       <c r="M181" s="22"/>
@@ -13528,7 +13554,7 @@
       <c r="G182" s="28"/>
       <c r="H182" s="28"/>
       <c r="I182" s="28"/>
-      <c r="J182" s="54"/>
+      <c r="J182" s="55"/>
       <c r="K182" s="23"/>
       <c r="L182" s="24"/>
       <c r="M182" s="22"/>
@@ -13545,12 +13571,46 @@
       <c r="G183" s="28"/>
       <c r="H183" s="28"/>
       <c r="I183" s="28"/>
-      <c r="J183" s="54"/>
+      <c r="J183" s="55"/>
       <c r="K183" s="23"/>
       <c r="L183" s="24"/>
       <c r="M183" s="22"/>
       <c r="N183" s="24"/>
       <c r="O183" s="23"/>
+    </row>
+    <row r="184" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+      <c r="A184" s="20"/>
+      <c r="B184" s="21"/>
+      <c r="C184" s="27"/>
+      <c r="D184" s="28"/>
+      <c r="E184" s="28"/>
+      <c r="F184" s="28"/>
+      <c r="G184" s="28"/>
+      <c r="H184" s="28"/>
+      <c r="I184" s="28"/>
+      <c r="J184" s="55"/>
+      <c r="K184" s="23"/>
+      <c r="L184" s="24"/>
+      <c r="M184" s="22"/>
+      <c r="N184" s="24"/>
+      <c r="O184" s="23"/>
+    </row>
+    <row r="185" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
+      <c r="A185" s="20"/>
+      <c r="B185" s="21"/>
+      <c r="C185" s="27"/>
+      <c r="D185" s="28"/>
+      <c r="E185" s="28"/>
+      <c r="F185" s="28"/>
+      <c r="G185" s="28"/>
+      <c r="H185" s="28"/>
+      <c r="I185" s="28"/>
+      <c r="J185" s="55"/>
+      <c r="K185" s="23"/>
+      <c r="L185" s="24"/>
+      <c r="M185" s="22"/>
+      <c r="N185" s="24"/>
+      <c r="O185" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -13559,18 +13619,18 @@
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="L2:O2"/>
   </mergeCells>
-  <conditionalFormatting sqref="N84:N183">
+  <conditionalFormatting sqref="N86:N185">
     <cfRule type="beginsWith" dxfId="0" priority="4" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N84,LEN("WARN"))="WARN"</formula>
+      <formula>LEFT(N86,LEN("WARN"))="WARN"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="5" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N84,LEN("FAIL"))="FAIL"</formula>
+      <formula>LEFT(N86,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="6" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N84,LEN("PASS"))="PASS"</formula>
+      <formula>LEFT(N86,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N1 N3:N83">
+  <conditionalFormatting sqref="N1 N3:N85">
     <cfRule type="beginsWith" dxfId="0" priority="7" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N1,LEN("WARN"))="WARN"</formula>
     </cfRule>
@@ -13582,10 +13642,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5 C6 C9 C10 C11 C12 C13 C14 C17 C18 C19 C20 C21 C22 C23 C24 C27 C28 C31 C32 C33 C34 C35 C36 C37 C38 C39 C43 C44 C45 C46 C49 C50 C51 C7:C8 C15:C16 C25:C26 C29:C30 C40:C42 C47:C48 C52:C183">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5 C6 C9 C10 C11 C12 C13 C14 C17 C18 C19 C20 C21 C22 C23 C24 C27 C28 C29 C30 C31 C32 C33 C34 C35 C36 C37 C38 C39 C40 C41 C45 C46 C47 C48 C51 C52 C53 C7:C8 C15:C16 C25:C26 C42:C44 C49:C50 C54:C185">
       <formula1>target</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5 D6 D9 D10 D11 D12 D13 D14 D17 D18 D19 D20 D21 D22 D23 D24 D25 D26 D27 D28 D31 D32 D33 D34 D35 D36 D37 D38 D39 D43 D44 D45 D46 D49 D50 D51 D7:D8 D15:D16 D29:D30 D40:D42 D47:D48 D52:D183">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5 D6 D9 D10 D11 D12 D13 D14 D17 D18 D19 D20 D21 D22 D23 D24 D25 D26 D27 D28 D29 D30 D31 D32 D33 D34 D35 D36 D37 D38 D39 D40 D41 D45 D46 D47 D48 D51 D52 D53 D7:D8 D15:D16 D42:D44 D49:D50 D54:D185">
       <formula1>INDIRECT(C5)</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>